<commit_message>
Ajout de la correction sur sprint2
</commit_message>
<xml_diff>
--- a/Equipe101.xlsx
+++ b/Equipe101.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23930"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{FA34F46B-4FBD-4D45-A4CE-032486D68F31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B19E26DB-CBBC-4D31-9241-F582E0DE6099}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{FA34F46B-4FBD-4D45-A4CE-032486D68F31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E4DBD59E-6AE5-4FB0-BC3C-0810670AC5FB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Sudoku" sheetId="1" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="196">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -2907,10 +2907,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="12" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="15" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2924,19 +2939,16 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="12" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2949,18 +2961,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5581,22 +5581,22 @@
       </c>
       <c r="B5" s="152">
         <f>(Fonctionnalités!E35)</f>
-        <v>0</v>
+        <v>0.95400000000000007</v>
       </c>
       <c r="C5" s="153">
         <f>'Assurance Qualité'!D60</f>
-        <v>0</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="D5" s="153">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0</v>
+        <v>0.85040000000000004</v>
       </c>
       <c r="F5" s="149">
         <v>25</v>
       </c>
       <c r="G5" s="150">
         <f>D5*F5</f>
-        <v>0</v>
+        <v>21.26</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1">
@@ -5648,8 +5648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J56"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5657,21 +5657,21 @@
     <col min="1" max="1" width="68.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="12.7109375" style="1" customWidth="1"/>
     <col min="4" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.7109375" customWidth="1"/>
+    <col min="10" max="11" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="296" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
+      <c r="B1" s="296"/>
+      <c r="C1" s="296"/>
+      <c r="D1" s="296"/>
+      <c r="E1" s="296"/>
+      <c r="F1" s="296"/>
+      <c r="G1" s="296"/>
       <c r="H1" s="160"/>
       <c r="I1" s="160"/>
     </row>
@@ -5680,15 +5680,15 @@
       <c r="I2" s="161"/>
     </row>
     <row r="3" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A3" s="291" t="s">
+      <c r="A3" s="290" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="291"/>
-      <c r="C3" s="291"/>
-      <c r="D3" s="291"/>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291"/>
+      <c r="B3" s="290"/>
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290"/>
       <c r="H3" s="162"/>
       <c r="I3" s="162"/>
     </row>
@@ -5704,31 +5704,31 @@
       <c r="I4" s="164"/>
     </row>
     <row r="5" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A5" s="292" t="s">
+      <c r="A5" s="297" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="293" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="293"/>
-      <c r="D5" s="294" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="294"/>
-      <c r="F5" s="295" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="295"/>
+      <c r="B5" s="298" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="298"/>
+      <c r="D5" s="299" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="299"/>
+      <c r="F5" s="300" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="300"/>
       <c r="H5" s="165"/>
       <c r="I5" s="165"/>
-      <c r="J5" s="299" t="s">
+      <c r="J5" s="294" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="299"/>
-      <c r="L5" s="299"/>
+      <c r="K5" s="294"/>
+      <c r="L5" s="294"/>
     </row>
     <row r="6" spans="1:13" ht="18.75">
-      <c r="A6" s="292"/>
+      <c r="A6" s="297"/>
       <c r="B6" s="166" t="s">
         <v>48</v>
       </c>
@@ -5761,20 +5761,23 @@
       <c r="M6" s="172"/>
     </row>
     <row r="7" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A7" s="291" t="s">
+      <c r="A7" s="290" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="291"/>
-      <c r="C7" s="291"/>
-      <c r="D7" s="291"/>
-      <c r="E7" s="291"/>
-      <c r="F7" s="291"/>
-      <c r="G7" s="291"/>
+      <c r="B7" s="290"/>
+      <c r="C7" s="290"/>
+      <c r="D7" s="290"/>
+      <c r="E7" s="290"/>
+      <c r="F7" s="290"/>
+      <c r="G7" s="290"/>
       <c r="H7" s="162" t="s">
         <v>84</v>
       </c>
       <c r="I7" s="162"/>
-      <c r="J7" s="300" t="s">
+      <c r="J7" s="295" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="295" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5788,7 +5791,9 @@
       <c r="C8" s="175">
         <v>3</v>
       </c>
-      <c r="D8" s="176"/>
+      <c r="D8" s="176">
+        <v>1</v>
+      </c>
       <c r="E8" s="175">
         <v>3</v>
       </c>
@@ -5798,7 +5803,8 @@
       </c>
       <c r="H8" s="178"/>
       <c r="I8" s="178"/>
-      <c r="J8" s="300"/>
+      <c r="J8" s="295"/>
+      <c r="K8" s="295"/>
     </row>
     <row r="9" spans="1:13" ht="60">
       <c r="A9" s="173" t="s">
@@ -5810,7 +5816,9 @@
       <c r="C9" s="180">
         <v>2</v>
       </c>
-      <c r="D9" s="181"/>
+      <c r="D9" s="181">
+        <v>1</v>
+      </c>
       <c r="E9" s="180">
         <v>2</v>
       </c>
@@ -5820,7 +5828,8 @@
       </c>
       <c r="H9" s="178"/>
       <c r="I9" s="178"/>
-      <c r="J9" s="300"/>
+      <c r="J9" s="295"/>
+      <c r="K9" s="295"/>
     </row>
     <row r="10" spans="1:13" ht="60">
       <c r="A10" s="183" t="s">
@@ -5832,7 +5841,9 @@
       <c r="C10" s="180">
         <v>3</v>
       </c>
-      <c r="D10" s="181"/>
+      <c r="D10" s="181">
+        <v>1</v>
+      </c>
       <c r="E10" s="180">
         <v>3</v>
       </c>
@@ -5842,7 +5853,8 @@
       </c>
       <c r="H10" s="178"/>
       <c r="I10" s="178"/>
-      <c r="J10" s="300"/>
+      <c r="J10" s="295"/>
+      <c r="K10" s="295"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="184" t="s">
@@ -5854,7 +5866,9 @@
       <c r="C11" s="180">
         <v>2</v>
       </c>
-      <c r="D11" s="181"/>
+      <c r="D11" s="181">
+        <v>0</v>
+      </c>
       <c r="E11" s="180">
         <v>2</v>
       </c>
@@ -5864,7 +5878,8 @@
       </c>
       <c r="H11" s="178"/>
       <c r="I11" s="178"/>
-      <c r="J11" s="300"/>
+      <c r="J11" s="295"/>
+      <c r="K11" s="295"/>
     </row>
     <row r="12" spans="1:13" ht="30">
       <c r="A12" s="185" t="s">
@@ -5876,7 +5891,9 @@
       <c r="C12" s="180">
         <v>4</v>
       </c>
-      <c r="D12" s="181"/>
+      <c r="D12" s="181">
+        <v>0</v>
+      </c>
       <c r="E12" s="180">
         <v>4</v>
       </c>
@@ -5886,7 +5903,8 @@
       </c>
       <c r="H12" s="178"/>
       <c r="I12" s="178"/>
-      <c r="J12" s="300"/>
+      <c r="J12" s="295"/>
+      <c r="K12" s="295"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="186" t="s">
@@ -5902,7 +5920,7 @@
       </c>
       <c r="D13" s="189">
         <f>SUMPRODUCT(D8:D12,E8:E12)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E13" s="190">
         <f>SUM(E8:E12)</f>
@@ -5918,23 +5936,25 @@
       </c>
       <c r="H13" s="178"/>
       <c r="I13" s="178"/>
-      <c r="J13" s="300"/>
+      <c r="J13" s="295"/>
+      <c r="K13" s="295"/>
     </row>
     <row r="14" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A14" s="291" t="s">
+      <c r="A14" s="290" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="291"/>
-      <c r="C14" s="291"/>
-      <c r="D14" s="291"/>
-      <c r="E14" s="291"/>
-      <c r="F14" s="291"/>
-      <c r="G14" s="291"/>
+      <c r="B14" s="290"/>
+      <c r="C14" s="290"/>
+      <c r="D14" s="290"/>
+      <c r="E14" s="290"/>
+      <c r="F14" s="290"/>
+      <c r="G14" s="290"/>
       <c r="H14" s="162" t="s">
         <v>84</v>
       </c>
       <c r="I14" s="162"/>
-      <c r="J14" s="300"/>
+      <c r="J14" s="295"/>
+      <c r="K14" s="295"/>
     </row>
     <row r="15" spans="1:13" ht="45">
       <c r="A15" s="183" t="s">
@@ -5946,7 +5966,9 @@
       <c r="C15" s="194">
         <v>2</v>
       </c>
-      <c r="D15" s="195"/>
+      <c r="D15" s="195">
+        <v>1</v>
+      </c>
       <c r="E15" s="194">
         <v>2</v>
       </c>
@@ -5956,7 +5978,8 @@
       </c>
       <c r="H15" s="197"/>
       <c r="I15" s="178"/>
-      <c r="J15" s="300"/>
+      <c r="J15" s="295"/>
+      <c r="K15" s="295"/>
     </row>
     <row r="16" spans="1:13" ht="30">
       <c r="A16" s="183" t="s">
@@ -5968,7 +5991,9 @@
       <c r="C16" s="199">
         <v>3</v>
       </c>
-      <c r="D16" s="200"/>
+      <c r="D16" s="200">
+        <v>1</v>
+      </c>
       <c r="E16" s="199">
         <v>3</v>
       </c>
@@ -5978,9 +6003,10 @@
       </c>
       <c r="H16" s="197"/>
       <c r="I16" s="178"/>
-      <c r="J16" s="300"/>
-    </row>
-    <row r="17" spans="1:10" ht="45">
+      <c r="J16" s="295"/>
+      <c r="K16" s="295"/>
+    </row>
+    <row r="17" spans="1:11" ht="45">
       <c r="A17" s="202" t="s">
         <v>95</v>
       </c>
@@ -5990,7 +6016,9 @@
       <c r="C17" s="199">
         <v>3</v>
       </c>
-      <c r="D17" s="203"/>
+      <c r="D17" s="203">
+        <v>0.5</v>
+      </c>
       <c r="E17" s="199">
         <v>3</v>
       </c>
@@ -6000,9 +6028,10 @@
       </c>
       <c r="H17" s="197"/>
       <c r="I17" s="178"/>
-      <c r="J17" s="300"/>
-    </row>
-    <row r="18" spans="1:10" ht="30">
+      <c r="J17" s="295"/>
+      <c r="K17" s="295"/>
+    </row>
+    <row r="18" spans="1:11" ht="30">
       <c r="A18" s="202" t="s">
         <v>96</v>
       </c>
@@ -6012,7 +6041,9 @@
       <c r="C18" s="199">
         <v>3</v>
       </c>
-      <c r="D18" s="203"/>
+      <c r="D18" s="203">
+        <v>1</v>
+      </c>
       <c r="E18" s="199">
         <v>3</v>
       </c>
@@ -6022,9 +6053,10 @@
       </c>
       <c r="H18" s="197"/>
       <c r="I18" s="178"/>
-      <c r="J18" s="300"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="J18" s="295"/>
+      <c r="K18" s="295"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="205" t="s">
         <v>97</v>
       </c>
@@ -6034,7 +6066,9 @@
       <c r="C19" s="199">
         <v>2</v>
       </c>
-      <c r="D19" s="207"/>
+      <c r="D19" s="207">
+        <v>0</v>
+      </c>
       <c r="E19" s="199">
         <v>2</v>
       </c>
@@ -6044,9 +6078,10 @@
       </c>
       <c r="H19" s="197"/>
       <c r="I19" s="178"/>
-      <c r="J19" s="300"/>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="J19" s="295"/>
+      <c r="K19" s="295"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="208" t="s">
         <v>91</v>
       </c>
@@ -6060,7 +6095,7 @@
       </c>
       <c r="D20" s="209">
         <f>SUMPRODUCT(D15:D19,E15:E19)</f>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="E20" s="210">
         <f>SUM(E15:E19)</f>
@@ -6076,25 +6111,27 @@
       </c>
       <c r="H20" s="197"/>
       <c r="I20" s="178"/>
-      <c r="J20" s="300"/>
-    </row>
-    <row r="21" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A21" s="291" t="s">
+      <c r="J20" s="295"/>
+      <c r="K20" s="295"/>
+    </row>
+    <row r="21" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A21" s="290" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="291"/>
-      <c r="C21" s="291"/>
-      <c r="D21" s="291"/>
-      <c r="E21" s="291"/>
-      <c r="F21" s="291"/>
-      <c r="G21" s="291"/>
+      <c r="B21" s="290"/>
+      <c r="C21" s="290"/>
+      <c r="D21" s="290"/>
+      <c r="E21" s="290"/>
+      <c r="F21" s="290"/>
+      <c r="G21" s="290"/>
       <c r="H21" s="162" t="s">
         <v>84</v>
       </c>
       <c r="I21" s="162"/>
-      <c r="J21" s="300"/>
-    </row>
-    <row r="22" spans="1:10" ht="75" customHeight="1">
+      <c r="J21" s="295"/>
+      <c r="K21" s="295"/>
+    </row>
+    <row r="22" spans="1:11" ht="75" customHeight="1">
       <c r="A22" s="184" t="s">
         <v>99</v>
       </c>
@@ -6104,7 +6141,9 @@
       <c r="C22" s="199">
         <v>2</v>
       </c>
-      <c r="D22" s="181"/>
+      <c r="D22" s="181">
+        <v>1</v>
+      </c>
       <c r="E22" s="199">
         <v>2</v>
       </c>
@@ -6114,9 +6153,10 @@
       </c>
       <c r="H22" s="197"/>
       <c r="I22" s="178"/>
-      <c r="J22" s="300"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="J22" s="295"/>
+      <c r="K22" s="295"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="185" t="s">
         <v>100</v>
       </c>
@@ -6126,7 +6166,9 @@
       <c r="C23" s="180">
         <v>1</v>
       </c>
-      <c r="D23" s="181"/>
+      <c r="D23" s="181">
+        <v>1</v>
+      </c>
       <c r="E23" s="180">
         <v>1</v>
       </c>
@@ -6136,9 +6178,10 @@
       </c>
       <c r="H23" s="197"/>
       <c r="I23" s="178"/>
-      <c r="J23" s="300"/>
-    </row>
-    <row r="24" spans="1:10" ht="30">
+      <c r="J23" s="295"/>
+      <c r="K23" s="295"/>
+    </row>
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="185" t="s">
         <v>101</v>
       </c>
@@ -6148,7 +6191,9 @@
       <c r="C24" s="180">
         <v>1</v>
       </c>
-      <c r="D24" s="181"/>
+      <c r="D24" s="181">
+        <v>1</v>
+      </c>
       <c r="E24" s="180">
         <v>1</v>
       </c>
@@ -6158,9 +6203,10 @@
       </c>
       <c r="H24" s="197"/>
       <c r="I24" s="178"/>
-      <c r="J24" s="300"/>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="J24" s="295"/>
+      <c r="K24" s="295"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="186" t="s">
         <v>91</v>
       </c>
@@ -6174,7 +6220,7 @@
       </c>
       <c r="D25" s="189">
         <f>SUMPRODUCT(D22:D24,E22:E24)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E25" s="190">
         <f>SUM(E22:E24)</f>
@@ -6190,25 +6236,27 @@
       </c>
       <c r="H25" s="197"/>
       <c r="I25" s="178"/>
-      <c r="J25" s="300"/>
-    </row>
-    <row r="26" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A26" s="291" t="s">
+      <c r="J25" s="295"/>
+      <c r="K25" s="295"/>
+    </row>
+    <row r="26" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A26" s="290" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="291"/>
-      <c r="C26" s="291"/>
-      <c r="D26" s="291"/>
-      <c r="E26" s="291"/>
-      <c r="F26" s="291"/>
-      <c r="G26" s="291"/>
+      <c r="B26" s="290"/>
+      <c r="C26" s="290"/>
+      <c r="D26" s="290"/>
+      <c r="E26" s="290"/>
+      <c r="F26" s="290"/>
+      <c r="G26" s="290"/>
       <c r="H26" s="162" t="s">
         <v>103</v>
       </c>
       <c r="I26" s="162"/>
-      <c r="J26" s="300"/>
-    </row>
-    <row r="27" spans="1:10" ht="60" customHeight="1">
+      <c r="J26" s="295"/>
+      <c r="K26" s="295"/>
+    </row>
+    <row r="27" spans="1:11" ht="60" customHeight="1">
       <c r="A27" s="205" t="s">
         <v>104</v>
       </c>
@@ -6218,7 +6266,9 @@
       <c r="C27" s="213">
         <v>2</v>
       </c>
-      <c r="D27" s="203"/>
+      <c r="D27" s="203">
+        <v>1</v>
+      </c>
       <c r="E27" s="213">
         <v>2</v>
       </c>
@@ -6228,9 +6278,10 @@
       </c>
       <c r="H27" s="197"/>
       <c r="I27" s="178"/>
-      <c r="J27" s="300"/>
-    </row>
-    <row r="28" spans="1:10" ht="45">
+      <c r="J27" s="295"/>
+      <c r="K27" s="295"/>
+    </row>
+    <row r="28" spans="1:11" ht="45">
       <c r="A28" s="205" t="s">
         <v>105</v>
       </c>
@@ -6240,7 +6291,9 @@
       <c r="C28" s="180">
         <v>2</v>
       </c>
-      <c r="D28" s="203"/>
+      <c r="D28" s="203">
+        <v>1</v>
+      </c>
       <c r="E28" s="180">
         <v>2</v>
       </c>
@@ -6250,9 +6303,10 @@
       </c>
       <c r="H28" s="197"/>
       <c r="I28" s="178"/>
-      <c r="J28" s="300"/>
-    </row>
-    <row r="29" spans="1:10" ht="30">
+      <c r="J28" s="295"/>
+      <c r="K28" s="295"/>
+    </row>
+    <row r="29" spans="1:11" ht="30">
       <c r="A29" s="205" t="s">
         <v>106</v>
       </c>
@@ -6262,7 +6316,9 @@
       <c r="C29" s="180">
         <v>2</v>
       </c>
-      <c r="D29" s="203"/>
+      <c r="D29" s="203">
+        <v>1</v>
+      </c>
       <c r="E29" s="180">
         <v>2</v>
       </c>
@@ -6272,9 +6328,10 @@
       </c>
       <c r="H29" s="197"/>
       <c r="I29" s="178"/>
-      <c r="J29" s="300"/>
-    </row>
-    <row r="30" spans="1:10" ht="75">
+      <c r="J29" s="295"/>
+      <c r="K29" s="295"/>
+    </row>
+    <row r="30" spans="1:11" ht="75">
       <c r="A30" s="205" t="s">
         <v>107</v>
       </c>
@@ -6284,7 +6341,9 @@
       <c r="C30" s="180">
         <v>3</v>
       </c>
-      <c r="D30" s="203"/>
+      <c r="D30" s="203">
+        <v>0.75</v>
+      </c>
       <c r="E30" s="180">
         <v>3</v>
       </c>
@@ -6294,9 +6353,10 @@
       </c>
       <c r="H30" s="197"/>
       <c r="I30" s="178"/>
-      <c r="J30" s="300"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="J30" s="295"/>
+      <c r="K30" s="295"/>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="208" t="s">
         <v>91</v>
       </c>
@@ -6310,7 +6370,7 @@
       </c>
       <c r="D31" s="209">
         <f>SUMPRODUCT(D27:D30,E27:E30)</f>
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="E31" s="190">
         <f>SUM(E27:E30)</f>
@@ -6326,25 +6386,27 @@
       </c>
       <c r="H31" s="197"/>
       <c r="I31" s="178"/>
-      <c r="J31" s="300"/>
-    </row>
-    <row r="32" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A32" s="291" t="s">
+      <c r="J31" s="295"/>
+      <c r="K31" s="295"/>
+    </row>
+    <row r="32" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A32" s="290" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="291"/>
-      <c r="C32" s="291"/>
-      <c r="D32" s="291"/>
-      <c r="E32" s="291"/>
-      <c r="F32" s="291"/>
-      <c r="G32" s="291"/>
+      <c r="B32" s="290"/>
+      <c r="C32" s="290"/>
+      <c r="D32" s="290"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
       <c r="H32" s="162" t="s">
         <v>103</v>
       </c>
       <c r="I32" s="162"/>
-      <c r="J32" s="300"/>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="J32" s="295"/>
+      <c r="K32" s="295"/>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="183" t="s">
         <v>109</v>
       </c>
@@ -6354,7 +6416,9 @@
       <c r="C33" s="213">
         <v>1</v>
       </c>
-      <c r="D33" s="215"/>
+      <c r="D33" s="215">
+        <v>1</v>
+      </c>
       <c r="E33" s="213">
         <v>1</v>
       </c>
@@ -6364,9 +6428,10 @@
       </c>
       <c r="H33" s="197"/>
       <c r="I33" s="178"/>
-      <c r="J33" s="300"/>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="J33" s="295"/>
+      <c r="K33" s="295"/>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="183" t="s">
         <v>110</v>
       </c>
@@ -6376,7 +6441,9 @@
       <c r="C34" s="199">
         <v>1</v>
       </c>
-      <c r="D34" s="203"/>
+      <c r="D34" s="203">
+        <v>1</v>
+      </c>
       <c r="E34" s="199">
         <v>1</v>
       </c>
@@ -6386,9 +6453,10 @@
       </c>
       <c r="H34" s="197"/>
       <c r="I34" s="178"/>
-      <c r="J34" s="300"/>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="J34" s="295"/>
+      <c r="K34" s="295"/>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="202" t="s">
         <v>111</v>
       </c>
@@ -6398,7 +6466,9 @@
       <c r="C35" s="199">
         <v>3</v>
       </c>
-      <c r="D35" s="203"/>
+      <c r="D35" s="203">
+        <v>0.75</v>
+      </c>
       <c r="E35" s="199">
         <v>3</v>
       </c>
@@ -6408,9 +6478,10 @@
       </c>
       <c r="H35" s="197"/>
       <c r="I35" s="178"/>
-      <c r="J35" s="300"/>
-    </row>
-    <row r="36" spans="1:10" ht="30">
+      <c r="J35" s="295"/>
+      <c r="K35" s="295"/>
+    </row>
+    <row r="36" spans="1:11" ht="30">
       <c r="A36" s="205" t="s">
         <v>112</v>
       </c>
@@ -6420,7 +6491,9 @@
       <c r="C36" s="180">
         <v>3</v>
       </c>
-      <c r="D36" s="203"/>
+      <c r="D36" s="203">
+        <v>1</v>
+      </c>
       <c r="E36" s="180">
         <v>3</v>
       </c>
@@ -6430,9 +6503,10 @@
       </c>
       <c r="H36" s="178"/>
       <c r="I36" s="178"/>
-      <c r="J36" s="300"/>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="J36" s="295"/>
+      <c r="K36" s="295"/>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="208" t="s">
         <v>91</v>
       </c>
@@ -6446,7 +6520,7 @@
       </c>
       <c r="D37" s="219">
         <f>SUMPRODUCT(D33:D36,E33:E36)</f>
-        <v>0</v>
+        <v>7.25</v>
       </c>
       <c r="E37" s="190">
         <f>SUM(E33:E36)</f>
@@ -6462,25 +6536,27 @@
       </c>
       <c r="H37" s="197"/>
       <c r="I37" s="178"/>
-      <c r="J37" s="300"/>
-    </row>
-    <row r="38" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A38" s="291" t="s">
+      <c r="J37" s="295"/>
+      <c r="K37" s="295"/>
+    </row>
+    <row r="38" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A38" s="290" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="291"/>
-      <c r="C38" s="291"/>
-      <c r="D38" s="291"/>
-      <c r="E38" s="291"/>
-      <c r="F38" s="291"/>
-      <c r="G38" s="291"/>
+      <c r="B38" s="290"/>
+      <c r="C38" s="290"/>
+      <c r="D38" s="290"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
       <c r="H38" s="162" t="s">
         <v>114</v>
       </c>
       <c r="I38" s="162"/>
-      <c r="J38" s="300"/>
-    </row>
-    <row r="39" spans="1:10" ht="45">
+      <c r="J38" s="295"/>
+      <c r="K38" s="295"/>
+    </row>
+    <row r="39" spans="1:11" ht="45">
       <c r="A39" s="202" t="s">
         <v>115</v>
       </c>
@@ -6490,7 +6566,9 @@
       <c r="C39" s="194">
         <v>1</v>
       </c>
-      <c r="D39" s="203"/>
+      <c r="D39" s="203">
+        <v>0.5</v>
+      </c>
       <c r="E39" s="194">
         <v>1</v>
       </c>
@@ -6500,9 +6578,10 @@
       </c>
       <c r="H39" s="178"/>
       <c r="I39" s="178"/>
-      <c r="J39" s="300"/>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="J39" s="295"/>
+      <c r="K39" s="295"/>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="202" t="s">
         <v>116</v>
       </c>
@@ -6512,7 +6591,9 @@
       <c r="C40" s="199">
         <v>4</v>
       </c>
-      <c r="D40" s="203"/>
+      <c r="D40" s="203">
+        <v>0.25</v>
+      </c>
       <c r="E40" s="199">
         <v>4</v>
       </c>
@@ -6522,9 +6603,10 @@
       </c>
       <c r="H40" s="178"/>
       <c r="I40" s="178"/>
-      <c r="J40" s="300"/>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="J40" s="295"/>
+      <c r="K40" s="295"/>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="202" t="s">
         <v>117</v>
       </c>
@@ -6534,7 +6616,9 @@
       <c r="C41" s="199">
         <v>3</v>
       </c>
-      <c r="D41" s="203"/>
+      <c r="D41" s="203">
+        <v>0.5</v>
+      </c>
       <c r="E41" s="199">
         <v>3</v>
       </c>
@@ -6544,9 +6628,10 @@
       </c>
       <c r="H41" s="178"/>
       <c r="I41" s="178"/>
-      <c r="J41" s="300"/>
-    </row>
-    <row r="42" spans="1:10" ht="60">
+      <c r="J41" s="295"/>
+      <c r="K41" s="295"/>
+    </row>
+    <row r="42" spans="1:11" ht="60">
       <c r="A42" s="202" t="s">
         <v>118</v>
       </c>
@@ -6556,7 +6641,9 @@
       <c r="C42" s="199">
         <v>2</v>
       </c>
-      <c r="D42" s="203"/>
+      <c r="D42" s="203">
+        <v>0.5</v>
+      </c>
       <c r="E42" s="199">
         <v>2</v>
       </c>
@@ -6565,9 +6652,10 @@
         <v>2</v>
       </c>
       <c r="H42" s="178"/>
-      <c r="J42" s="300"/>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="J42" s="295"/>
+      <c r="K42" s="295"/>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="202" t="s">
         <v>119</v>
       </c>
@@ -6577,7 +6665,9 @@
       <c r="C43" s="199">
         <v>2</v>
       </c>
-      <c r="D43" s="203"/>
+      <c r="D43" s="203">
+        <v>0.25</v>
+      </c>
       <c r="E43" s="199">
         <v>2</v>
       </c>
@@ -6587,9 +6677,10 @@
       </c>
       <c r="H43" s="178"/>
       <c r="I43" s="178"/>
-      <c r="J43" s="300"/>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="J43" s="295"/>
+      <c r="K43" s="295"/>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="202" t="s">
         <v>120</v>
       </c>
@@ -6599,7 +6690,9 @@
       <c r="C44" s="199">
         <v>3</v>
       </c>
-      <c r="D44" s="203"/>
+      <c r="D44" s="203">
+        <v>1</v>
+      </c>
       <c r="E44" s="199">
         <v>3</v>
       </c>
@@ -6609,9 +6702,10 @@
       </c>
       <c r="H44" s="178"/>
       <c r="I44" s="178"/>
-      <c r="J44" s="300"/>
-    </row>
-    <row r="45" spans="1:10" ht="30">
+      <c r="J44" s="295"/>
+      <c r="K44" s="295"/>
+    </row>
+    <row r="45" spans="1:11" ht="30">
       <c r="A45" s="202" t="s">
         <v>121</v>
       </c>
@@ -6621,7 +6715,9 @@
       <c r="C45" s="199">
         <v>3</v>
       </c>
-      <c r="D45" s="203"/>
+      <c r="D45" s="203">
+        <v>0.5</v>
+      </c>
       <c r="E45" s="199">
         <v>3</v>
       </c>
@@ -6631,9 +6727,10 @@
       </c>
       <c r="H45" s="178"/>
       <c r="I45" s="178"/>
-      <c r="J45" s="300"/>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="J45" s="295"/>
+      <c r="K45" s="295"/>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="202" t="s">
         <v>122</v>
       </c>
@@ -6643,7 +6740,9 @@
       <c r="C46" s="199">
         <v>4</v>
       </c>
-      <c r="D46" s="203"/>
+      <c r="D46" s="203">
+        <v>1</v>
+      </c>
       <c r="E46" s="199">
         <v>4</v>
       </c>
@@ -6653,9 +6752,10 @@
       </c>
       <c r="H46" s="178"/>
       <c r="I46" s="178"/>
-      <c r="J46" s="300"/>
-    </row>
-    <row r="47" spans="1:10" ht="60">
+      <c r="J46" s="295"/>
+      <c r="K46" s="295"/>
+    </row>
+    <row r="47" spans="1:11" ht="60">
       <c r="A47" s="205" t="s">
         <v>123</v>
       </c>
@@ -6665,7 +6765,9 @@
       <c r="C47" s="180">
         <v>10</v>
       </c>
-      <c r="D47" s="203"/>
+      <c r="D47" s="203">
+        <v>0.25</v>
+      </c>
       <c r="E47" s="180">
         <v>10</v>
       </c>
@@ -6675,9 +6777,10 @@
       </c>
       <c r="H47" s="178"/>
       <c r="I47" s="178"/>
-      <c r="J47" s="300"/>
-    </row>
-    <row r="48" spans="1:10" ht="30">
+      <c r="J47" s="295"/>
+      <c r="K47" s="295"/>
+    </row>
+    <row r="48" spans="1:11" ht="30">
       <c r="A48" s="205" t="s">
         <v>124</v>
       </c>
@@ -6687,7 +6790,9 @@
       <c r="C48" s="180">
         <v>6</v>
       </c>
-      <c r="D48" s="203"/>
+      <c r="D48" s="203">
+        <v>0.5</v>
+      </c>
       <c r="E48" s="180">
         <v>6</v>
       </c>
@@ -6697,9 +6802,10 @@
       </c>
       <c r="H48" s="178"/>
       <c r="I48" s="178"/>
-      <c r="J48" s="300"/>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="J48" s="295"/>
+      <c r="K48" s="295"/>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="205" t="s">
         <v>125</v>
       </c>
@@ -6709,7 +6815,9 @@
       <c r="C49" s="180">
         <v>3</v>
       </c>
-      <c r="D49" s="203"/>
+      <c r="D49" s="203">
+        <v>1</v>
+      </c>
       <c r="E49" s="180">
         <v>3</v>
       </c>
@@ -6719,9 +6827,10 @@
       </c>
       <c r="H49" s="178"/>
       <c r="I49" s="178"/>
-      <c r="J49" s="300"/>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="J49" s="295"/>
+      <c r="K49" s="295"/>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="208" t="s">
         <v>91</v>
       </c>
@@ -6735,7 +6844,7 @@
       </c>
       <c r="D50" s="219">
         <f>SUMPRODUCT(D39:D49,E39:E49)</f>
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="E50" s="190">
         <f>SUM(E39:E49)</f>
@@ -6751,25 +6860,27 @@
       </c>
       <c r="H50" s="197"/>
       <c r="I50" s="178"/>
-      <c r="J50" s="300"/>
-    </row>
-    <row r="51" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A51" s="291" t="s">
+      <c r="J50" s="295"/>
+      <c r="K50" s="295"/>
+    </row>
+    <row r="51" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A51" s="290" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="291"/>
-      <c r="C51" s="291"/>
-      <c r="D51" s="291"/>
-      <c r="E51" s="291"/>
-      <c r="F51" s="291"/>
-      <c r="G51" s="291"/>
+      <c r="B51" s="290"/>
+      <c r="C51" s="290"/>
+      <c r="D51" s="290"/>
+      <c r="E51" s="290"/>
+      <c r="F51" s="290"/>
+      <c r="G51" s="290"/>
       <c r="H51" s="162" t="s">
         <v>103</v>
       </c>
       <c r="I51" s="162"/>
-      <c r="J51" s="300"/>
-    </row>
-    <row r="52" spans="1:10" ht="30">
+      <c r="J51" s="295"/>
+      <c r="K51" s="295"/>
+    </row>
+    <row r="52" spans="1:11" ht="30">
       <c r="A52" s="220" t="s">
         <v>127</v>
       </c>
@@ -6779,7 +6890,9 @@
       <c r="C52" s="221">
         <v>2</v>
       </c>
-      <c r="D52" s="222"/>
+      <c r="D52" s="222">
+        <v>1</v>
+      </c>
       <c r="E52" s="221">
         <v>2</v>
       </c>
@@ -6789,9 +6902,10 @@
       </c>
       <c r="H52" s="197"/>
       <c r="I52" s="178"/>
-      <c r="J52" s="300"/>
-    </row>
-    <row r="53" spans="1:10" ht="30">
+      <c r="J52" s="295"/>
+      <c r="K52" s="295"/>
+    </row>
+    <row r="53" spans="1:11" ht="30">
       <c r="A53" s="185" t="s">
         <v>128</v>
       </c>
@@ -6801,7 +6915,9 @@
       <c r="C53" s="180">
         <v>2</v>
       </c>
-      <c r="D53" s="224"/>
+      <c r="D53" s="224">
+        <v>1</v>
+      </c>
       <c r="E53" s="180">
         <v>2</v>
       </c>
@@ -6811,9 +6927,10 @@
       </c>
       <c r="H53" s="178"/>
       <c r="I53" s="178"/>
-      <c r="J53" s="300"/>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="J53" s="295"/>
+      <c r="K53" s="295"/>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="185" t="s">
         <v>129</v>
       </c>
@@ -6823,7 +6940,9 @@
       <c r="C54" s="180">
         <v>1</v>
       </c>
-      <c r="D54" s="203"/>
+      <c r="D54" s="203">
+        <v>1</v>
+      </c>
       <c r="E54" s="180">
         <v>1</v>
       </c>
@@ -6833,9 +6952,10 @@
       </c>
       <c r="H54" s="178"/>
       <c r="I54" s="178"/>
-      <c r="J54" s="300"/>
-    </row>
-    <row r="55" spans="1:10" ht="120" customHeight="1">
+      <c r="J54" s="295"/>
+      <c r="K54" s="295"/>
+    </row>
+    <row r="55" spans="1:11" ht="120" customHeight="1">
       <c r="A55" s="185" t="s">
         <v>130</v>
       </c>
@@ -6845,7 +6965,9 @@
       <c r="C55" s="180">
         <v>4</v>
       </c>
-      <c r="D55" s="203"/>
+      <c r="D55" s="203">
+        <v>1</v>
+      </c>
       <c r="E55" s="180">
         <v>4</v>
       </c>
@@ -6855,9 +6977,10 @@
       </c>
       <c r="H55" s="178"/>
       <c r="I55" s="178"/>
-      <c r="J55" s="300"/>
-    </row>
-    <row r="56" spans="1:10" ht="45">
+      <c r="J55" s="295"/>
+      <c r="K55" s="295"/>
+    </row>
+    <row r="56" spans="1:11" ht="45">
       <c r="A56" s="184" t="s">
         <v>131</v>
       </c>
@@ -6867,7 +6990,9 @@
       <c r="C56" s="199">
         <v>2</v>
       </c>
-      <c r="D56" s="280"/>
+      <c r="D56" s="280">
+        <v>1</v>
+      </c>
       <c r="E56" s="199">
         <v>2</v>
       </c>
@@ -6877,9 +7002,10 @@
       </c>
       <c r="H56" s="226"/>
       <c r="I56" s="178"/>
-      <c r="J56" s="300"/>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="J56" s="295"/>
+      <c r="K56" s="295"/>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="227" t="s">
         <v>91</v>
       </c>
@@ -6893,7 +7019,7 @@
       </c>
       <c r="D57" s="189">
         <f>SUMPRODUCT(D52:D56,E52:E56)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E57" s="190">
         <f>SUM(E52:E56)</f>
@@ -6910,20 +7036,20 @@
       <c r="H57" s="178"/>
       <c r="I57" s="178"/>
     </row>
-    <row r="58" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A58" s="291" t="s">
+    <row r="58" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A58" s="290" t="s">
         <v>76</v>
       </c>
-      <c r="B58" s="291"/>
-      <c r="C58" s="291"/>
-      <c r="D58" s="291"/>
-      <c r="E58" s="291"/>
-      <c r="F58" s="291"/>
-      <c r="G58" s="291"/>
+      <c r="B58" s="290"/>
+      <c r="C58" s="290"/>
+      <c r="D58" s="290"/>
+      <c r="E58" s="290"/>
+      <c r="F58" s="290"/>
+      <c r="G58" s="290"/>
       <c r="H58" s="162"/>
       <c r="I58" s="162"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:11">
       <c r="A59" s="230" t="s">
         <v>132</v>
       </c>
@@ -6937,7 +7063,7 @@
       </c>
       <c r="D59" s="232">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>69.5</v>
       </c>
       <c r="E59" s="233">
         <f t="shared" si="0"/>
@@ -6954,30 +7080,36 @@
       <c r="H59" s="226"/>
       <c r="I59" s="178"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:11">
       <c r="A60" s="230" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="296">
+      <c r="B60" s="291">
         <f>B59/C59</f>
         <v>0.82</v>
       </c>
-      <c r="C60" s="296"/>
-      <c r="D60" s="297">
+      <c r="C60" s="291"/>
+      <c r="D60" s="292">
         <f>D59/E59</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="297"/>
-      <c r="F60" s="298">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="E60" s="292"/>
+      <c r="F60" s="293">
         <f>F59/G59</f>
         <v>0</v>
       </c>
-      <c r="G60" s="298"/>
+      <c r="G60" s="293"/>
       <c r="H60" s="236"/>
       <c r="I60" s="236"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="D60:E60"/>
@@ -6991,12 +7123,7 @@
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="A38:G38"/>
     <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="K7:K56"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13 H20 H25 H31 H37 H50" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -7786,8 +7913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H34" sqref="H24:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7802,14 +7929,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="301" t="s">
+      <c r="A1" s="305" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
+      <c r="B1" s="305"/>
+      <c r="C1" s="305"/>
+      <c r="D1" s="305"/>
+      <c r="E1" s="305"/>
+      <c r="F1" s="305"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="283"/>
@@ -7820,34 +7947,34 @@
       <c r="F2" s="237"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="301" t="s">
+      <c r="A3" s="305" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="301"/>
-      <c r="C3" s="301"/>
-      <c r="D3" s="301"/>
-      <c r="E3" s="301"/>
-      <c r="F3" s="301"/>
+      <c r="B3" s="305"/>
+      <c r="C3" s="305"/>
+      <c r="D3" s="305"/>
+      <c r="E3" s="305"/>
+      <c r="F3" s="305"/>
     </row>
     <row r="5" spans="1:8" ht="23.25">
-      <c r="A5" s="302" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="302"/>
-      <c r="C5" s="302"/>
-      <c r="D5" s="302"/>
-      <c r="E5" s="302"/>
-      <c r="F5" s="302"/>
+      <c r="A5" s="306" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="306"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="306"/>
+      <c r="E5" s="306"/>
+      <c r="F5" s="306"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="238" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="303"/>
-      <c r="C6" s="303"/>
-      <c r="D6" s="303"/>
-      <c r="E6" s="303"/>
-      <c r="F6" s="303"/>
+      <c r="B6" s="307"/>
+      <c r="C6" s="307"/>
+      <c r="D6" s="307"/>
+      <c r="E6" s="307"/>
+      <c r="F6" s="307"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="239" t="s">
@@ -7890,7 +8017,7 @@
       <c r="G8" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="300" t="s">
+      <c r="H8" s="295" t="s">
         <v>85</v>
       </c>
     </row>
@@ -7915,7 +8042,7 @@
       <c r="G9" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="300"/>
+      <c r="H9" s="295"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="242" t="s">
@@ -7938,7 +8065,7 @@
       <c r="G10" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="300"/>
+      <c r="H10" s="295"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="242" t="s">
@@ -7961,7 +8088,7 @@
       <c r="G11" t="s">
         <v>84</v>
       </c>
-      <c r="H11" s="300"/>
+      <c r="H11" s="295"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="242" t="s">
@@ -7984,7 +8111,7 @@
       <c r="G12" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="300"/>
+      <c r="H12" s="295"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="242" t="s">
@@ -8007,7 +8134,7 @@
       <c r="G13" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="300"/>
+      <c r="H13" s="295"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="242" t="s">
@@ -8030,7 +8157,7 @@
       <c r="G14" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="300"/>
+      <c r="H14" s="295"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="242" t="s">
@@ -8053,7 +8180,7 @@
       <c r="G15" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="300"/>
+      <c r="H15" s="295"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="242" t="s">
@@ -8076,7 +8203,7 @@
       <c r="G16" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="300"/>
+      <c r="H16" s="295"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="242" t="s">
@@ -8099,14 +8226,14 @@
       <c r="G17" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="300"/>
+      <c r="H17" s="295"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="246" t="s">
         <v>171</v>
       </c>
-      <c r="B18" s="304"/>
-      <c r="C18" s="304"/>
+      <c r="B18" s="308"/>
+      <c r="C18" s="308"/>
       <c r="D18" s="284">
         <f>SUM(D8:D17)</f>
         <v>100</v>
@@ -8134,24 +8261,24 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="23.25" customHeight="1">
-      <c r="A21" s="305" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="305"/>
-      <c r="C21" s="305"/>
-      <c r="D21" s="305"/>
-      <c r="E21" s="305"/>
-      <c r="F21" s="305"/>
+      <c r="A21" s="301" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="301"/>
+      <c r="C21" s="301"/>
+      <c r="D21" s="301"/>
+      <c r="E21" s="301"/>
+      <c r="F21" s="301"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="251" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="306"/>
-      <c r="C22" s="306"/>
-      <c r="D22" s="306"/>
-      <c r="E22" s="306"/>
-      <c r="F22" s="306"/>
+      <c r="B22" s="302"/>
+      <c r="C22" s="302"/>
+      <c r="D22" s="302"/>
+      <c r="E22" s="302"/>
+      <c r="F22" s="302"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="251" t="s">
@@ -8173,172 +8300,262 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="25.5" customHeight="1">
+    <row r="24" spans="1:8">
       <c r="A24" s="251" t="s">
         <v>174</v>
       </c>
-      <c r="B24" s="253"/>
-      <c r="C24" s="253"/>
+      <c r="B24" s="253">
+        <v>1</v>
+      </c>
+      <c r="C24" s="253">
+        <v>1</v>
+      </c>
       <c r="D24" s="251">
         <v>8</v>
       </c>
       <c r="E24" s="251">
         <f t="shared" ref="E24:E34" si="1">B24*C24*D24</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F24" s="252"/>
+      <c r="G24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="295" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="251" t="s">
         <v>175</v>
       </c>
-      <c r="B25" s="253"/>
-      <c r="C25" s="253"/>
+      <c r="B25" s="253">
+        <v>1</v>
+      </c>
+      <c r="C25" s="253">
+        <v>1</v>
+      </c>
       <c r="D25" s="251">
         <v>16</v>
       </c>
       <c r="E25" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F25" s="252"/>
+      <c r="G25" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="295"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="251" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="253"/>
-      <c r="C26" s="253"/>
+      <c r="B26" s="253">
+        <v>1</v>
+      </c>
+      <c r="C26" s="253">
+        <v>1</v>
+      </c>
       <c r="D26" s="251">
         <v>8</v>
       </c>
       <c r="E26" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F26" s="252"/>
+      <c r="G26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="295"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="251" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="253"/>
-      <c r="C27" s="253"/>
+      <c r="B27" s="253">
+        <v>1</v>
+      </c>
+      <c r="C27" s="253">
+        <v>1</v>
+      </c>
       <c r="D27" s="251">
         <v>6</v>
       </c>
       <c r="E27" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F27" s="252"/>
+      <c r="G27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="295"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="251" t="s">
         <v>178</v>
       </c>
-      <c r="B28" s="253"/>
-      <c r="C28" s="253"/>
+      <c r="B28" s="253">
+        <v>1</v>
+      </c>
+      <c r="C28" s="253">
+        <v>1</v>
+      </c>
       <c r="D28" s="251">
         <v>8</v>
       </c>
       <c r="E28" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F28" s="252"/>
+      <c r="G28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="295"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="251" t="s">
         <v>179</v>
       </c>
-      <c r="B29" s="253"/>
-      <c r="C29" s="253"/>
+      <c r="B29" s="253">
+        <v>1</v>
+      </c>
+      <c r="C29" s="253">
+        <v>1</v>
+      </c>
       <c r="D29" s="251">
         <v>10</v>
       </c>
       <c r="E29" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F29" s="252"/>
+      <c r="G29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="295"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="251" t="s">
         <v>180</v>
       </c>
-      <c r="B30" s="253"/>
-      <c r="C30" s="253"/>
+      <c r="B30" s="253">
+        <v>1</v>
+      </c>
+      <c r="C30" s="253">
+        <v>1</v>
+      </c>
       <c r="D30" s="251">
         <v>8</v>
       </c>
       <c r="E30" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F30" s="252"/>
+      <c r="G30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="295"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="251" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="253"/>
-      <c r="C31" s="253"/>
+      <c r="B31" s="253">
+        <v>1</v>
+      </c>
+      <c r="C31" s="253">
+        <v>1</v>
+      </c>
       <c r="D31" s="251">
         <v>8</v>
       </c>
       <c r="E31" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F31" s="252"/>
+      <c r="G31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" s="295"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="251" t="s">
         <v>182</v>
       </c>
-      <c r="B32" s="253"/>
-      <c r="C32" s="253"/>
+      <c r="B32" s="253">
+        <v>0.9</v>
+      </c>
+      <c r="C32" s="253">
+        <v>0.75</v>
+      </c>
       <c r="D32" s="251">
         <v>8</v>
       </c>
       <c r="E32" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.4</v>
       </c>
       <c r="F32" s="252"/>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" s="295"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="251" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="253"/>
-      <c r="C33" s="253"/>
+      <c r="B33" s="253">
+        <v>1</v>
+      </c>
+      <c r="C33" s="253">
+        <v>0.75</v>
+      </c>
       <c r="D33" s="251">
         <v>8</v>
       </c>
       <c r="E33" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F33" s="252"/>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="295"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="251" t="s">
         <v>184</v>
       </c>
-      <c r="B34" s="253"/>
-      <c r="C34" s="253"/>
+      <c r="B34" s="253">
+        <v>1</v>
+      </c>
+      <c r="C34" s="253">
+        <v>1</v>
+      </c>
       <c r="D34" s="251">
         <v>12</v>
       </c>
       <c r="E34" s="251">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F34" s="252"/>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" s="295"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="254" t="s">
         <v>171</v>
       </c>
@@ -8350,11 +8567,11 @@
       </c>
       <c r="E35" s="256">
         <f>SUM(E24:E34)/D35 -E36*D36 -E37*D37-E38*D38</f>
-        <v>0</v>
+        <v>0.95400000000000007</v>
       </c>
       <c r="F35" s="257"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:8">
       <c r="A36" s="258" t="s">
         <v>172</v>
       </c>
@@ -8363,7 +8580,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:8">
       <c r="A37" s="258" t="s">
         <v>173</v>
       </c>
@@ -8371,7 +8588,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:8">
       <c r="A38" s="258" t="s">
         <v>185</v>
       </c>
@@ -8379,27 +8596,27 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="23.25">
-      <c r="A39" s="307" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="307"/>
-      <c r="C39" s="307"/>
-      <c r="D39" s="307"/>
-      <c r="E39" s="307"/>
-      <c r="F39" s="307"/>
-    </row>
-    <row r="40" spans="1:6">
+    <row r="39" spans="1:8" ht="23.25">
+      <c r="A39" s="303" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="303"/>
+      <c r="C39" s="303"/>
+      <c r="D39" s="303"/>
+      <c r="E39" s="303"/>
+      <c r="F39" s="303"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="263" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="308"/>
-      <c r="C40" s="308"/>
-      <c r="D40" s="308"/>
-      <c r="E40" s="308"/>
-      <c r="F40" s="308"/>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="B40" s="304"/>
+      <c r="C40" s="304"/>
+      <c r="D40" s="304"/>
+      <c r="E40" s="304"/>
+      <c r="F40" s="304"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="264" t="s">
         <v>158</v>
       </c>
@@ -8419,7 +8636,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:8">
       <c r="A42" s="267" t="s">
         <v>186</v>
       </c>
@@ -8434,7 +8651,7 @@
       </c>
       <c r="F42" s="266"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:8">
       <c r="A43" s="267" t="s">
         <v>187</v>
       </c>
@@ -8449,7 +8666,7 @@
       </c>
       <c r="F43" s="266"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:8">
       <c r="A44" s="267" t="s">
         <v>188</v>
       </c>
@@ -8464,7 +8681,7 @@
       </c>
       <c r="F44" s="269"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:8">
       <c r="A45" s="267" t="s">
         <v>189</v>
       </c>
@@ -8479,7 +8696,7 @@
       </c>
       <c r="F45" s="266"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:8">
       <c r="A46" s="267" t="s">
         <v>190</v>
       </c>
@@ -8494,7 +8711,7 @@
       </c>
       <c r="F46" s="266"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:8">
       <c r="A47" s="267" t="s">
         <v>191</v>
       </c>
@@ -8509,7 +8726,7 @@
       </c>
       <c r="F47" s="266"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:8">
       <c r="A48" s="270" t="s">
         <v>192</v>
       </c>
@@ -8610,17 +8827,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="H8:H17"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H24:H34"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B18 B42:B51" xr:uid="{00000000-0002-0000-0700-000000000000}">

</xml_diff>

<commit_message>
Ajout de la correction du sprint 3
</commit_message>
<xml_diff>
--- a/Equipe101.xlsx
+++ b/Equipe101.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{FA34F46B-4FBD-4D45-A4CE-032486D68F31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B19E26DB-CBBC-4D31-9241-F582E0DE6099}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="13_ncr:1_{FA34F46B-4FBD-4D45-A4CE-032486D68F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BF65C1A-F635-4DA8-AF77-EB5F697C20FF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Old Sudoku" sheetId="1" state="hidden" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Curling" sheetId="9" state="hidden" r:id="rId8"/>
     <sheet name="Fonctionnalités" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="196">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -2183,7 +2183,7 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="309">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2310,7 +2310,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2381,13 +2381,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="36" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2414,8 +2414,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="10" borderId="51" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="9" fontId="0" fillId="11" borderId="52" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2452,7 +2452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2462,9 +2462,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1"/>
@@ -2504,7 +2501,7 @@
     <xf numFmtId="10" fontId="5" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2513,7 +2510,7 @@
     <xf numFmtId="10" fontId="5" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="71" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2522,20 +2519,19 @@
     <xf numFmtId="10" fontId="0" fillId="8" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2556,10 +2552,10 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2574,7 +2570,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2589,16 +2585,16 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="15" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="76" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="64" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2619,43 +2615,34 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="82" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="83" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="84" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="75" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2664,7 +2651,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="85" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="15" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="82" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="86" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2673,9 +2660,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2700,7 +2684,7 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="86" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="88" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="89" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2718,10 +2702,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="83" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="15" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="90" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="91" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2730,7 +2714,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2754,19 +2738,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="94" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2787,14 +2771,14 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2812,7 +2796,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1"/>
@@ -2825,7 +2809,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="96" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2834,10 +2818,10 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="94" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2846,7 +2830,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="75" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="97" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2870,48 +2854,54 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="82" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="82" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="82" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="88" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="12" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="15" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2923,33 +2913,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="10" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="12" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="92" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2961,6 +2924,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="92" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3821,18 +3796,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
-      <c r="C2" s="285" t="s">
+      <c r="C2" s="277" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="285"/>
-      <c r="E2" s="286" t="s">
+      <c r="D2" s="277"/>
+      <c r="E2" s="278" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="286"/>
-      <c r="G2" s="287" t="s">
+      <c r="F2" s="278"/>
+      <c r="G2" s="279" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="287"/>
+      <c r="H2" s="279"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2"/>
@@ -4112,7 +4087,7 @@
       <c r="F2" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="288" t="s">
+      <c r="G2" s="280" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4125,7 +4100,7 @@
       <c r="D3" s="55"/>
       <c r="E3" s="56"/>
       <c r="F3" s="57"/>
-      <c r="G3" s="288"/>
+      <c r="G3" s="280"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="58" t="s">
@@ -4385,7 +4360,6 @@
         <f>SUMPRODUCT(F$4:F$21,$G$4:$G$21)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="161"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="85" t="s">
@@ -4411,7 +4385,6 @@
         <f>SUMPRODUCT(--ISNUMBER(F$4:F$21),$G$4:$G$21)</f>
         <v>0</v>
       </c>
-      <c r="G23" s="161"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="91" t="s">
@@ -4442,15 +4415,10 @@
       <c r="A27" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="161"/>
-      <c r="C27" s="161"/>
-      <c r="D27" s="161"/>
-      <c r="E27" s="161"/>
-      <c r="F27" s="161"/>
-      <c r="H27" s="289" t="s">
+      <c r="H27" s="281" t="s">
         <v>55</v>
       </c>
-      <c r="I27" s="289"/>
+      <c r="I27" s="281"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="52" t="s">
@@ -4653,24 +4621,16 @@
         <f>IF(F$28="Oui",$H$37,$I$37)</f>
         <v>10</v>
       </c>
-      <c r="H38" s="136"/>
-      <c r="I38" s="136"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="137"/>
-      <c r="B39" s="137"/>
-      <c r="C39" s="137"/>
-      <c r="D39" s="137"/>
-      <c r="E39" s="137"/>
-      <c r="F39" s="137"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="161"/>
-      <c r="B40" s="161"/>
-      <c r="C40" s="161"/>
-      <c r="D40" s="161"/>
-      <c r="E40" s="161"/>
-      <c r="F40" s="161"/>
+      <c r="A39" s="136"/>
+      <c r="B39" s="136"/>
+      <c r="C39" s="136"/>
+      <c r="D39" s="136"/>
+      <c r="E39" s="136"/>
+      <c r="F39" s="136"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="91" t="s">
@@ -4701,7 +4661,7 @@
       <c r="A44" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="138">
+      <c r="B44" s="137">
         <f>(B$25+B$41)/2</f>
         <v>0.5</v>
       </c>
@@ -4726,23 +4686,23 @@
       <c r="A45" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="139">
+      <c r="B45" s="138">
         <f>COUNTA(B$4:B$21)</f>
         <v>0</v>
       </c>
-      <c r="C45" s="140">
+      <c r="C45" s="139">
         <f>COUNTA(C$4:C$21)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="141">
+      <c r="D45" s="140">
         <f>COUNTA(D$4:D$21)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="142">
+      <c r="E45" s="141">
         <f>COUNTA(E$4:E$21)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="143">
+      <c r="F45" s="142">
         <f>COUNTA(F$4:F$21)</f>
         <v>0</v>
       </c>
@@ -4803,7 +4763,7 @@
       <c r="F2" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="288" t="s">
+      <c r="G2" s="280" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4816,7 +4776,7 @@
       <c r="D3" s="55"/>
       <c r="E3" s="56"/>
       <c r="F3" s="57"/>
-      <c r="G3" s="288"/>
+      <c r="G3" s="280"/>
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="58" t="s">
@@ -5128,7 +5088,6 @@
         <f>SUMPRODUCT(F$4:F$25,$G$4:$G$25)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="161"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="85" t="s">
@@ -5154,7 +5113,6 @@
         <f>SUMPRODUCT(--ISNUMBER(F$4:F$25),$G$4:$G$25)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="161"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="91" t="s">
@@ -5185,15 +5143,10 @@
       <c r="A31" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="161"/>
-      <c r="C31" s="161"/>
-      <c r="D31" s="161"/>
-      <c r="E31" s="161"/>
-      <c r="F31" s="161"/>
-      <c r="H31" s="289" t="s">
+      <c r="H31" s="281" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="289"/>
+      <c r="I31" s="281"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="52" t="s">
@@ -5396,24 +5349,16 @@
         <f>IF(F$32="Oui",$H$41,$I$41)</f>
         <v>10</v>
       </c>
-      <c r="H42" s="136"/>
-      <c r="I42" s="136"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="137"/>
-      <c r="B43" s="137"/>
-      <c r="C43" s="137"/>
-      <c r="D43" s="137"/>
-      <c r="E43" s="137"/>
-      <c r="F43" s="137"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="161"/>
-      <c r="B44" s="161"/>
-      <c r="C44" s="161"/>
-      <c r="D44" s="161"/>
-      <c r="E44" s="161"/>
-      <c r="F44" s="161"/>
+      <c r="A43" s="136"/>
+      <c r="B43" s="136"/>
+      <c r="C43" s="136"/>
+      <c r="D43" s="136"/>
+      <c r="E43" s="136"/>
+      <c r="F43" s="136"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="91" t="s">
@@ -5444,7 +5389,7 @@
       <c r="A48" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="138">
+      <c r="B48" s="137">
         <f>(B$29+B$45)/2</f>
         <v>0.5</v>
       </c>
@@ -5469,23 +5414,23 @@
       <c r="A49" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="139">
+      <c r="B49" s="138">
         <f>COUNTA(B$4:B$25)</f>
         <v>0</v>
       </c>
-      <c r="C49" s="140">
+      <c r="C49" s="139">
         <f>COUNTA(C$4:C$25)</f>
         <v>0</v>
       </c>
-      <c r="D49" s="141">
+      <c r="D49" s="140">
         <f>COUNTA(D$4:D$25)</f>
         <v>0</v>
       </c>
-      <c r="E49" s="142">
+      <c r="E49" s="141">
         <f>COUNTA(E$4:E$25)</f>
         <v>0</v>
       </c>
-      <c r="F49" s="143">
+      <c r="F49" s="142">
         <f>COUNTA(F$4:F$25)</f>
         <v>0</v>
       </c>
@@ -5516,7 +5461,7 @@
   <dimension ref="A3:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5531,17 +5476,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7">
-      <c r="A3" s="283"/>
-      <c r="B3" s="144" t="s">
+      <c r="A3" s="170"/>
+      <c r="B3" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="143" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="143" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="145" t="s">
+      <c r="E3" s="144" t="s">
         <v>77</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -5552,90 +5497,92 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="146" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="147">
+      <c r="A4" s="145" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="146">
         <f>(Fonctionnalités!E18)</f>
         <v>0.94879999999999998</v>
       </c>
-      <c r="C4" s="148">
+      <c r="C4" s="147">
         <f>'Assurance Qualité'!B60</f>
         <v>0.82</v>
       </c>
-      <c r="D4" s="148">
+      <c r="D4" s="147">
         <f>B4*0.6+C4*0.4 - 0.1*E4</f>
         <v>0.89728000000000008</v>
       </c>
-      <c r="F4" s="149">
+      <c r="F4" s="148">
         <v>15</v>
       </c>
-      <c r="G4" s="150">
+      <c r="G4" s="149">
         <f>D4*F4</f>
         <v>13.459200000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="151" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="152">
+      <c r="A5" s="150" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="151">
         <f>(Fonctionnalités!E35)</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="153">
+        <v>0.98</v>
+      </c>
+      <c r="C5" s="152">
         <f>'Assurance Qualité'!D60</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="153">
+        <v>0.71</v>
+      </c>
+      <c r="D5" s="152">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="149">
+        <v>0.87199999999999989</v>
+      </c>
+      <c r="F5" s="148">
         <v>25</v>
       </c>
-      <c r="G5" s="150">
+      <c r="G5" s="149">
         <f>D5*F5</f>
-        <v>0</v>
+        <v>21.799999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A6" s="154" t="s">
+      <c r="A6" s="153" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="155">
+      <c r="B6" s="154">
         <f>(Fonctionnalités!E52)</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="156">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="C6" s="155">
         <f>'Assurance Qualité'!F60</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="156">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="D6" s="155">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="149">
+        <v>0.94216000000000011</v>
+      </c>
+      <c r="F6" s="148">
         <v>20</v>
       </c>
-      <c r="G6" s="150">
+      <c r="G6" s="149">
         <f>D6*F6</f>
-        <v>0</v>
+        <v>18.843200000000003</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A7" s="157" t="s">
+      <c r="A7" s="156" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="158"/>
-      <c r="C7" s="158"/>
-      <c r="D7" s="159"/>
+      <c r="B7" s="157"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="158">
+        <v>1</v>
+      </c>
       <c r="F7" s="2">
         <v>10</v>
       </c>
-      <c r="G7" s="150">
+      <c r="G7" s="149">
         <f>D7*F7</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5648,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J56"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5657,1327 +5604,1529 @@
     <col min="1" max="1" width="68.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="12.7109375" style="1" customWidth="1"/>
     <col min="4" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.7109375" customWidth="1"/>
+    <col min="10" max="11" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="287" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="H2" s="161"/>
-      <c r="I2" s="161"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="159"/>
     </row>
     <row r="3" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A3" s="291" t="s">
+      <c r="A3" s="282" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="291"/>
-      <c r="C3" s="291"/>
-      <c r="D3" s="291"/>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
+      <c r="B3" s="282"/>
+      <c r="C3" s="282"/>
+      <c r="D3" s="282"/>
+      <c r="E3" s="282"/>
+      <c r="F3" s="282"/>
+      <c r="G3" s="282"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
     </row>
     <row r="4" spans="1:13" ht="18.75">
-      <c r="A4" s="163"/>
-      <c r="B4" s="164"/>
-      <c r="C4" s="164"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="164"/>
-      <c r="G4" s="164"/>
-      <c r="H4" s="164"/>
-      <c r="I4" s="164"/>
+      <c r="A4" s="161"/>
+      <c r="B4" s="162"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="E4" s="162"/>
+      <c r="F4" s="162"/>
+      <c r="G4" s="162"/>
+      <c r="H4" s="162"/>
+      <c r="I4" s="162"/>
     </row>
     <row r="5" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A5" s="292" t="s">
+      <c r="A5" s="288" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="293" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="293"/>
-      <c r="D5" s="294" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="294"/>
-      <c r="F5" s="295" t="s">
+      <c r="B5" s="289" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="289"/>
+      <c r="D5" s="290" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="290"/>
+      <c r="F5" s="291" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="295"/>
-      <c r="H5" s="165"/>
-      <c r="I5" s="165"/>
-      <c r="J5" s="299" t="s">
+      <c r="G5" s="291"/>
+      <c r="H5" s="163"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="286" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="299"/>
-      <c r="L5" s="299"/>
+      <c r="K5" s="286"/>
+      <c r="L5" s="286"/>
     </row>
     <row r="6" spans="1:13" ht="18.75">
-      <c r="A6" s="292"/>
-      <c r="B6" s="166" t="s">
+      <c r="A6" s="288"/>
+      <c r="B6" s="164" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="167" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="168" t="s">
+      <c r="C6" s="165" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="166" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="169" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="170" t="s">
+      <c r="E6" s="167" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="168" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="171" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="165"/>
-      <c r="I6" s="165"/>
-      <c r="J6" s="172" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="172" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="172" t="s">
+      <c r="G6" s="169" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="170" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="170" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="170" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="172"/>
+      <c r="M6" s="170"/>
     </row>
     <row r="7" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A7" s="291" t="s">
+      <c r="A7" s="282" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="291"/>
-      <c r="C7" s="291"/>
-      <c r="D7" s="291"/>
-      <c r="E7" s="291"/>
-      <c r="F7" s="291"/>
-      <c r="G7" s="291"/>
-      <c r="H7" s="162" t="s">
+      <c r="B7" s="282"/>
+      <c r="C7" s="282"/>
+      <c r="D7" s="282"/>
+      <c r="E7" s="282"/>
+      <c r="F7" s="282"/>
+      <c r="G7" s="282"/>
+      <c r="H7" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="162"/>
-      <c r="J7" s="300" t="s">
+      <c r="I7" s="160"/>
+      <c r="J7" s="286" t="s">
         <v>85</v>
       </c>
+      <c r="K7" s="286" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="171" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="174">
-        <v>1</v>
-      </c>
-      <c r="C8" s="175">
-        <v>3</v>
-      </c>
-      <c r="D8" s="176"/>
-      <c r="E8" s="175">
-        <v>3</v>
-      </c>
-      <c r="F8" s="177"/>
-      <c r="G8" s="175">
-        <v>3</v>
-      </c>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="300"/>
-    </row>
-    <row r="9" spans="1:13" ht="60">
-      <c r="A9" s="173" t="s">
+      <c r="B8" s="172">
+        <v>1</v>
+      </c>
+      <c r="C8" s="173">
+        <v>3</v>
+      </c>
+      <c r="D8" s="174">
+        <v>1</v>
+      </c>
+      <c r="E8" s="173">
+        <v>3</v>
+      </c>
+      <c r="F8" s="175">
+        <v>1</v>
+      </c>
+      <c r="G8" s="173">
+        <v>3</v>
+      </c>
+      <c r="H8" s="176"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="286"/>
+      <c r="K8" s="286"/>
+    </row>
+    <row r="9" spans="1:13" ht="45">
+      <c r="A9" s="171" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="179">
-        <v>1</v>
-      </c>
-      <c r="C9" s="180">
+      <c r="B9" s="177">
+        <v>1</v>
+      </c>
+      <c r="C9" s="178">
         <v>2</v>
       </c>
-      <c r="D9" s="181"/>
-      <c r="E9" s="180">
+      <c r="D9" s="179">
+        <v>1</v>
+      </c>
+      <c r="E9" s="178">
         <v>2</v>
       </c>
-      <c r="F9" s="182"/>
-      <c r="G9" s="180">
+      <c r="F9" s="180">
+        <v>1</v>
+      </c>
+      <c r="G9" s="178">
         <v>2</v>
       </c>
-      <c r="H9" s="178"/>
-      <c r="I9" s="178"/>
-      <c r="J9" s="300"/>
-    </row>
-    <row r="10" spans="1:13" ht="60">
-      <c r="A10" s="183" t="s">
+      <c r="H9" s="176"/>
+      <c r="I9" s="176"/>
+      <c r="J9" s="286"/>
+      <c r="K9" s="286"/>
+    </row>
+    <row r="10" spans="1:13" ht="45">
+      <c r="A10" s="181" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="179">
-        <v>1</v>
-      </c>
-      <c r="C10" s="180">
-        <v>3</v>
-      </c>
-      <c r="D10" s="181"/>
-      <c r="E10" s="180">
-        <v>3</v>
-      </c>
-      <c r="F10" s="182"/>
-      <c r="G10" s="180">
-        <v>3</v>
-      </c>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="300"/>
+      <c r="B10" s="177">
+        <v>1</v>
+      </c>
+      <c r="C10" s="178">
+        <v>3</v>
+      </c>
+      <c r="D10" s="179">
+        <v>1</v>
+      </c>
+      <c r="E10" s="178">
+        <v>3</v>
+      </c>
+      <c r="F10" s="180">
+        <v>1</v>
+      </c>
+      <c r="G10" s="178">
+        <v>3</v>
+      </c>
+      <c r="H10" s="176"/>
+      <c r="I10" s="176"/>
+      <c r="J10" s="286"/>
+      <c r="K10" s="286"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="184" t="s">
+      <c r="A11" s="182" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="179">
+      <c r="B11" s="177">
         <v>0.5</v>
       </c>
-      <c r="C11" s="180">
+      <c r="C11" s="178">
         <v>2</v>
       </c>
-      <c r="D11" s="181"/>
-      <c r="E11" s="180">
+      <c r="D11" s="179">
+        <v>0</v>
+      </c>
+      <c r="E11" s="178">
         <v>2</v>
       </c>
-      <c r="F11" s="182"/>
-      <c r="G11" s="180">
+      <c r="F11" s="180">
+        <v>1</v>
+      </c>
+      <c r="G11" s="178">
         <v>2</v>
       </c>
-      <c r="H11" s="178"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="300"/>
+      <c r="H11" s="176"/>
+      <c r="I11" s="176"/>
+      <c r="J11" s="286"/>
+      <c r="K11" s="286"/>
     </row>
     <row r="12" spans="1:13" ht="30">
-      <c r="A12" s="185" t="s">
+      <c r="A12" s="183" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="179">
-        <v>0</v>
-      </c>
-      <c r="C12" s="180">
+      <c r="B12" s="177">
+        <v>0</v>
+      </c>
+      <c r="C12" s="178">
         <v>4</v>
       </c>
-      <c r="D12" s="181"/>
-      <c r="E12" s="180">
+      <c r="D12" s="179">
+        <v>0</v>
+      </c>
+      <c r="E12" s="178">
         <v>4</v>
       </c>
-      <c r="F12" s="182"/>
-      <c r="G12" s="180">
+      <c r="F12" s="180">
+        <v>0</v>
+      </c>
+      <c r="G12" s="178">
         <v>4</v>
       </c>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="300"/>
+      <c r="H12" s="176"/>
+      <c r="I12" s="176"/>
+      <c r="J12" s="286"/>
+      <c r="K12" s="286"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="186" t="s">
+      <c r="A13" s="184" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="187">
+      <c r="B13" s="185">
         <f>SUMPRODUCT(B8:B12,C8:C12)</f>
         <v>9</v>
       </c>
-      <c r="C13" s="188">
+      <c r="C13" s="186">
         <f>SUM(C8:C12)</f>
         <v>14</v>
       </c>
-      <c r="D13" s="189">
+      <c r="D13" s="187">
         <f>SUMPRODUCT(D8:D12,E8:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="190">
+        <v>8</v>
+      </c>
+      <c r="E13" s="188">
         <f>SUM(E8:E12)</f>
         <v>14</v>
       </c>
-      <c r="F13" s="191">
+      <c r="F13" s="189">
         <f>SUMPRODUCT(F8:F12,G8:G12)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="192">
+        <v>10</v>
+      </c>
+      <c r="G13" s="190">
         <f>SUM(G8:G12)</f>
         <v>14</v>
       </c>
-      <c r="H13" s="178"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="300"/>
+      <c r="H13" s="176"/>
+      <c r="I13" s="176"/>
+      <c r="J13" s="286"/>
+      <c r="K13" s="286"/>
     </row>
     <row r="14" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A14" s="291" t="s">
+      <c r="A14" s="282" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="291"/>
-      <c r="C14" s="291"/>
-      <c r="D14" s="291"/>
-      <c r="E14" s="291"/>
-      <c r="F14" s="291"/>
-      <c r="G14" s="291"/>
-      <c r="H14" s="162" t="s">
+      <c r="B14" s="282"/>
+      <c r="C14" s="282"/>
+      <c r="D14" s="282"/>
+      <c r="E14" s="282"/>
+      <c r="F14" s="282"/>
+      <c r="G14" s="282"/>
+      <c r="H14" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="162"/>
-      <c r="J14" s="300"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="286"/>
+      <c r="K14" s="286"/>
     </row>
     <row r="15" spans="1:13" ht="45">
-      <c r="A15" s="183" t="s">
+      <c r="A15" s="181" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="193">
+      <c r="B15" s="172">
         <v>0.5</v>
       </c>
-      <c r="C15" s="194">
+      <c r="C15" s="191">
         <v>2</v>
       </c>
-      <c r="D15" s="195"/>
-      <c r="E15" s="194">
+      <c r="D15" s="192">
+        <v>1</v>
+      </c>
+      <c r="E15" s="191">
         <v>2</v>
       </c>
-      <c r="F15" s="196"/>
-      <c r="G15" s="194">
+      <c r="F15" s="175">
+        <v>1</v>
+      </c>
+      <c r="G15" s="191">
         <v>2</v>
       </c>
-      <c r="H15" s="197"/>
-      <c r="I15" s="178"/>
-      <c r="J15" s="300"/>
+      <c r="H15" s="176"/>
+      <c r="I15" s="176"/>
+      <c r="J15" s="286"/>
+      <c r="K15" s="286"/>
     </row>
     <row r="16" spans="1:13" ht="30">
-      <c r="A16" s="183" t="s">
+      <c r="A16" s="181" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="198">
-        <v>1</v>
-      </c>
-      <c r="C16" s="199">
-        <v>3</v>
-      </c>
-      <c r="D16" s="200"/>
-      <c r="E16" s="199">
-        <v>3</v>
-      </c>
-      <c r="F16" s="201"/>
-      <c r="G16" s="199">
-        <v>3</v>
-      </c>
-      <c r="H16" s="197"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="300"/>
-    </row>
-    <row r="17" spans="1:10" ht="45">
-      <c r="A17" s="202" t="s">
+      <c r="B16" s="193">
+        <v>1</v>
+      </c>
+      <c r="C16" s="194">
+        <v>3</v>
+      </c>
+      <c r="D16" s="195">
+        <v>1</v>
+      </c>
+      <c r="E16" s="194">
+        <v>3</v>
+      </c>
+      <c r="F16" s="196">
+        <v>1</v>
+      </c>
+      <c r="G16" s="194">
+        <v>3</v>
+      </c>
+      <c r="H16" s="176"/>
+      <c r="I16" s="176"/>
+      <c r="J16" s="286"/>
+      <c r="K16" s="286"/>
+    </row>
+    <row r="17" spans="1:11" ht="45">
+      <c r="A17" s="197" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="179">
-        <v>0</v>
-      </c>
-      <c r="C17" s="199">
-        <v>3</v>
-      </c>
-      <c r="D17" s="203"/>
-      <c r="E17" s="199">
-        <v>3</v>
-      </c>
-      <c r="F17" s="204"/>
-      <c r="G17" s="199">
-        <v>3</v>
-      </c>
-      <c r="H17" s="197"/>
-      <c r="I17" s="178"/>
-      <c r="J17" s="300"/>
-    </row>
-    <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="202" t="s">
+      <c r="B17" s="177">
+        <v>0</v>
+      </c>
+      <c r="C17" s="194">
+        <v>3</v>
+      </c>
+      <c r="D17" s="198">
+        <v>1</v>
+      </c>
+      <c r="E17" s="194">
+        <v>3</v>
+      </c>
+      <c r="F17" s="199">
+        <v>1</v>
+      </c>
+      <c r="G17" s="194">
+        <v>3</v>
+      </c>
+      <c r="H17" s="176"/>
+      <c r="I17" s="176"/>
+      <c r="J17" s="286"/>
+      <c r="K17" s="286"/>
+    </row>
+    <row r="18" spans="1:11" ht="30">
+      <c r="A18" s="197" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="179">
-        <v>1</v>
-      </c>
-      <c r="C18" s="199">
-        <v>3</v>
-      </c>
-      <c r="D18" s="203"/>
-      <c r="E18" s="199">
-        <v>3</v>
-      </c>
-      <c r="F18" s="204"/>
-      <c r="G18" s="199">
-        <v>3</v>
-      </c>
-      <c r="H18" s="197"/>
-      <c r="I18" s="178"/>
-      <c r="J18" s="300"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="205" t="s">
+      <c r="B18" s="177">
+        <v>1</v>
+      </c>
+      <c r="C18" s="194">
+        <v>3</v>
+      </c>
+      <c r="D18" s="198">
+        <v>1</v>
+      </c>
+      <c r="E18" s="194">
+        <v>3</v>
+      </c>
+      <c r="F18" s="199">
+        <v>1</v>
+      </c>
+      <c r="G18" s="194">
+        <v>3</v>
+      </c>
+      <c r="H18" s="176"/>
+      <c r="I18" s="176"/>
+      <c r="J18" s="286"/>
+      <c r="K18" s="286"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="200" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="206">
-        <v>0</v>
-      </c>
-      <c r="C19" s="199">
+      <c r="B19" s="201">
+        <v>0</v>
+      </c>
+      <c r="C19" s="194">
         <v>2</v>
       </c>
-      <c r="D19" s="207"/>
-      <c r="E19" s="199">
+      <c r="D19" s="202">
+        <v>0</v>
+      </c>
+      <c r="E19" s="194">
         <v>2</v>
       </c>
-      <c r="F19" s="204"/>
-      <c r="G19" s="199">
+      <c r="F19" s="199">
+        <v>1</v>
+      </c>
+      <c r="G19" s="194">
         <v>2</v>
       </c>
-      <c r="H19" s="197"/>
-      <c r="I19" s="178"/>
-      <c r="J19" s="300"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="208" t="s">
+      <c r="H19" s="176"/>
+      <c r="I19" s="176"/>
+      <c r="J19" s="286"/>
+      <c r="K19" s="286"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="187">
+      <c r="B20" s="185">
         <f>SUMPRODUCT(B15:B19,C15:C19)</f>
         <v>7</v>
       </c>
-      <c r="C20" s="188">
+      <c r="C20" s="186">
         <f>SUM(C15:C19)</f>
         <v>13</v>
       </c>
-      <c r="D20" s="209">
+      <c r="D20" s="204">
         <f>SUMPRODUCT(D15:D19,E15:E19)</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="210">
+        <v>11</v>
+      </c>
+      <c r="E20" s="205">
         <f>SUM(E15:E19)</f>
         <v>13</v>
       </c>
-      <c r="F20" s="211">
+      <c r="F20" s="189">
         <f>SUMPRODUCT(F15:F19,G15:G19)</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="192">
+        <v>13</v>
+      </c>
+      <c r="G20" s="190">
         <f>SUM(G15:G19)</f>
         <v>13</v>
       </c>
-      <c r="H20" s="197"/>
-      <c r="I20" s="178"/>
-      <c r="J20" s="300"/>
-    </row>
-    <row r="21" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A21" s="291" t="s">
+      <c r="H20" s="176"/>
+      <c r="I20" s="176"/>
+      <c r="J20" s="286"/>
+      <c r="K20" s="286"/>
+    </row>
+    <row r="21" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A21" s="282" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="291"/>
-      <c r="C21" s="291"/>
-      <c r="D21" s="291"/>
-      <c r="E21" s="291"/>
-      <c r="F21" s="291"/>
-      <c r="G21" s="291"/>
-      <c r="H21" s="162" t="s">
+      <c r="B21" s="282"/>
+      <c r="C21" s="282"/>
+      <c r="D21" s="282"/>
+      <c r="E21" s="282"/>
+      <c r="F21" s="282"/>
+      <c r="G21" s="282"/>
+      <c r="H21" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="162"/>
-      <c r="J21" s="300"/>
-    </row>
-    <row r="22" spans="1:10" ht="75" customHeight="1">
-      <c r="A22" s="184" t="s">
+      <c r="I21" s="160"/>
+      <c r="J21" s="286"/>
+      <c r="K21" s="286"/>
+    </row>
+    <row r="22" spans="1:11" ht="75" customHeight="1">
+      <c r="A22" s="182" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="179">
-        <v>1</v>
-      </c>
-      <c r="C22" s="199">
+      <c r="B22" s="177">
+        <v>1</v>
+      </c>
+      <c r="C22" s="194">
         <v>2</v>
       </c>
-      <c r="D22" s="181"/>
-      <c r="E22" s="199">
+      <c r="D22" s="179">
+        <v>1</v>
+      </c>
+      <c r="E22" s="194">
         <v>2</v>
       </c>
-      <c r="F22" s="182"/>
-      <c r="G22" s="199">
+      <c r="F22" s="180">
+        <v>1</v>
+      </c>
+      <c r="G22" s="194">
         <v>2</v>
       </c>
-      <c r="H22" s="197"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="300"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="185" t="s">
+      <c r="H22" s="176"/>
+      <c r="I22" s="176"/>
+      <c r="J22" s="286"/>
+      <c r="K22" s="286"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="183" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="179">
-        <v>1</v>
-      </c>
-      <c r="C23" s="180">
-        <v>1</v>
-      </c>
-      <c r="D23" s="181"/>
-      <c r="E23" s="180">
-        <v>1</v>
-      </c>
-      <c r="F23" s="182"/>
-      <c r="G23" s="180">
-        <v>1</v>
-      </c>
-      <c r="H23" s="197"/>
-      <c r="I23" s="178"/>
-      <c r="J23" s="300"/>
-    </row>
-    <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="185" t="s">
+      <c r="B23" s="177">
+        <v>1</v>
+      </c>
+      <c r="C23" s="178">
+        <v>1</v>
+      </c>
+      <c r="D23" s="179">
+        <v>1</v>
+      </c>
+      <c r="E23" s="178">
+        <v>1</v>
+      </c>
+      <c r="F23" s="180">
+        <v>1</v>
+      </c>
+      <c r="G23" s="178">
+        <v>1</v>
+      </c>
+      <c r="H23" s="176"/>
+      <c r="I23" s="176"/>
+      <c r="J23" s="286"/>
+      <c r="K23" s="286"/>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="183" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="179">
-        <v>1</v>
-      </c>
-      <c r="C24" s="180">
-        <v>1</v>
-      </c>
-      <c r="D24" s="181"/>
-      <c r="E24" s="180">
-        <v>1</v>
-      </c>
-      <c r="F24" s="182"/>
-      <c r="G24" s="180">
-        <v>1</v>
-      </c>
-      <c r="H24" s="197"/>
-      <c r="I24" s="178"/>
-      <c r="J24" s="300"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="186" t="s">
+      <c r="B24" s="177">
+        <v>1</v>
+      </c>
+      <c r="C24" s="178">
+        <v>1</v>
+      </c>
+      <c r="D24" s="179">
+        <v>1</v>
+      </c>
+      <c r="E24" s="178">
+        <v>1</v>
+      </c>
+      <c r="F24" s="180">
+        <v>1</v>
+      </c>
+      <c r="G24" s="178">
+        <v>1</v>
+      </c>
+      <c r="H24" s="176"/>
+      <c r="I24" s="176"/>
+      <c r="J24" s="286"/>
+      <c r="K24" s="286"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="184" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="187">
+      <c r="B25" s="185">
         <f>SUMPRODUCT(B22:B24,C22:C24)</f>
         <v>4</v>
       </c>
-      <c r="C25" s="188">
+      <c r="C25" s="186">
         <f>SUM(C22:C24)</f>
         <v>4</v>
       </c>
-      <c r="D25" s="189">
+      <c r="D25" s="187">
         <f>SUMPRODUCT(D22:D24,E22:E24)</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="190">
+        <v>4</v>
+      </c>
+      <c r="E25" s="188">
         <f>SUM(E22:E24)</f>
         <v>4</v>
       </c>
-      <c r="F25" s="191">
+      <c r="F25" s="189">
         <f>SUMPRODUCT(F22:F24,G22:G24)</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="192">
+        <v>4</v>
+      </c>
+      <c r="G25" s="190">
         <f>SUM(G22:G24)</f>
         <v>4</v>
       </c>
-      <c r="H25" s="197"/>
-      <c r="I25" s="178"/>
-      <c r="J25" s="300"/>
-    </row>
-    <row r="26" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A26" s="291" t="s">
+      <c r="H25" s="176"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="286"/>
+      <c r="K25" s="286"/>
+    </row>
+    <row r="26" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A26" s="282" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="291"/>
-      <c r="C26" s="291"/>
-      <c r="D26" s="291"/>
-      <c r="E26" s="291"/>
-      <c r="F26" s="291"/>
-      <c r="G26" s="291"/>
-      <c r="H26" s="162" t="s">
+      <c r="B26" s="282"/>
+      <c r="C26" s="282"/>
+      <c r="D26" s="282"/>
+      <c r="E26" s="282"/>
+      <c r="F26" s="282"/>
+      <c r="G26" s="282"/>
+      <c r="H26" s="160" t="s">
         <v>103</v>
       </c>
-      <c r="I26" s="162"/>
-      <c r="J26" s="300"/>
-    </row>
-    <row r="27" spans="1:10" ht="60" customHeight="1">
-      <c r="A27" s="205" t="s">
+      <c r="I26" s="160"/>
+      <c r="J26" s="286"/>
+      <c r="K26" s="286"/>
+    </row>
+    <row r="27" spans="1:11" ht="60" customHeight="1">
+      <c r="A27" s="200" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="212">
-        <v>1</v>
-      </c>
-      <c r="C27" s="213">
+      <c r="B27" s="206">
+        <v>1</v>
+      </c>
+      <c r="C27" s="207">
         <v>2</v>
       </c>
-      <c r="D27" s="203"/>
-      <c r="E27" s="213">
+      <c r="D27" s="198">
+        <v>1</v>
+      </c>
+      <c r="E27" s="207">
         <v>2</v>
       </c>
-      <c r="F27" s="214"/>
-      <c r="G27" s="213">
+      <c r="F27" s="208">
+        <v>1</v>
+      </c>
+      <c r="G27" s="207">
         <v>2</v>
       </c>
-      <c r="H27" s="197"/>
-      <c r="I27" s="178"/>
-      <c r="J27" s="300"/>
-    </row>
-    <row r="28" spans="1:10" ht="45">
-      <c r="A28" s="205" t="s">
+      <c r="H27" s="176"/>
+      <c r="I27" s="176"/>
+      <c r="J27" s="286"/>
+      <c r="K27" s="286"/>
+    </row>
+    <row r="28" spans="1:11" ht="45">
+      <c r="A28" s="200" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="179">
-        <v>1</v>
-      </c>
-      <c r="C28" s="180">
+      <c r="B28" s="177">
+        <v>1</v>
+      </c>
+      <c r="C28" s="178">
         <v>2</v>
       </c>
-      <c r="D28" s="203"/>
-      <c r="E28" s="180">
+      <c r="D28" s="198">
+        <v>1</v>
+      </c>
+      <c r="E28" s="178">
         <v>2</v>
       </c>
-      <c r="F28" s="214"/>
-      <c r="G28" s="180">
+      <c r="F28" s="208">
+        <v>1</v>
+      </c>
+      <c r="G28" s="178">
         <v>2</v>
       </c>
-      <c r="H28" s="197"/>
-      <c r="I28" s="178"/>
-      <c r="J28" s="300"/>
-    </row>
-    <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="205" t="s">
+      <c r="H28" s="176"/>
+      <c r="I28" s="176"/>
+      <c r="J28" s="286"/>
+      <c r="K28" s="286"/>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" s="200" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="179">
-        <v>1</v>
-      </c>
-      <c r="C29" s="180">
+      <c r="B29" s="177">
+        <v>1</v>
+      </c>
+      <c r="C29" s="178">
         <v>2</v>
       </c>
-      <c r="D29" s="203"/>
-      <c r="E29" s="180">
+      <c r="D29" s="198">
+        <v>1</v>
+      </c>
+      <c r="E29" s="178">
         <v>2</v>
       </c>
-      <c r="F29" s="214"/>
-      <c r="G29" s="180">
+      <c r="F29" s="208">
+        <v>1</v>
+      </c>
+      <c r="G29" s="178">
         <v>2</v>
       </c>
-      <c r="H29" s="197"/>
-      <c r="I29" s="178"/>
-      <c r="J29" s="300"/>
-    </row>
-    <row r="30" spans="1:10" ht="75">
-      <c r="A30" s="205" t="s">
+      <c r="H29" s="176"/>
+      <c r="I29" s="176"/>
+      <c r="J29" s="286"/>
+      <c r="K29" s="286"/>
+    </row>
+    <row r="30" spans="1:11" ht="75">
+      <c r="A30" s="200" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="179">
-        <v>1</v>
-      </c>
-      <c r="C30" s="180">
-        <v>3</v>
-      </c>
-      <c r="D30" s="203"/>
-      <c r="E30" s="180">
-        <v>3</v>
-      </c>
-      <c r="F30" s="214"/>
-      <c r="G30" s="180">
-        <v>3</v>
-      </c>
-      <c r="H30" s="197"/>
-      <c r="I30" s="178"/>
-      <c r="J30" s="300"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="208" t="s">
+      <c r="B30" s="177">
+        <v>1</v>
+      </c>
+      <c r="C30" s="178">
+        <v>3</v>
+      </c>
+      <c r="D30" s="198">
+        <v>0.75</v>
+      </c>
+      <c r="E30" s="178">
+        <v>3</v>
+      </c>
+      <c r="F30" s="208">
+        <v>1</v>
+      </c>
+      <c r="G30" s="178">
+        <v>3</v>
+      </c>
+      <c r="H30" s="176"/>
+      <c r="I30" s="176"/>
+      <c r="J30" s="286"/>
+      <c r="K30" s="286"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="187">
+      <c r="B31" s="185">
         <f>SUMPRODUCT(B27:B30,C27:C30)</f>
         <v>9</v>
       </c>
-      <c r="C31" s="188">
+      <c r="C31" s="186">
         <f>SUM(C27:C30)</f>
         <v>9</v>
       </c>
-      <c r="D31" s="209">
+      <c r="D31" s="204">
         <f>SUMPRODUCT(D27:D30,E27:E30)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="190">
+        <v>8.25</v>
+      </c>
+      <c r="E31" s="188">
         <f>SUM(E27:E30)</f>
         <v>9</v>
       </c>
-      <c r="F31" s="191">
+      <c r="F31" s="189">
         <f>SUMPRODUCT(F27:F30,G27:G30)</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="192">
+        <v>9</v>
+      </c>
+      <c r="G31" s="190">
         <f>SUM(G27:G30)</f>
         <v>9</v>
       </c>
-      <c r="H31" s="197"/>
-      <c r="I31" s="178"/>
-      <c r="J31" s="300"/>
-    </row>
-    <row r="32" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A32" s="291" t="s">
+      <c r="H31" s="176"/>
+      <c r="I31" s="176"/>
+      <c r="J31" s="286"/>
+      <c r="K31" s="286"/>
+    </row>
+    <row r="32" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A32" s="282" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="291"/>
-      <c r="C32" s="291"/>
-      <c r="D32" s="291"/>
-      <c r="E32" s="291"/>
-      <c r="F32" s="291"/>
-      <c r="G32" s="291"/>
-      <c r="H32" s="162" t="s">
+      <c r="B32" s="282"/>
+      <c r="C32" s="282"/>
+      <c r="D32" s="282"/>
+      <c r="E32" s="282"/>
+      <c r="F32" s="282"/>
+      <c r="G32" s="282"/>
+      <c r="H32" s="160" t="s">
         <v>103</v>
       </c>
-      <c r="I32" s="162"/>
-      <c r="J32" s="300"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="183" t="s">
+      <c r="I32" s="160"/>
+      <c r="J32" s="286"/>
+      <c r="K32" s="286"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="181" t="s">
         <v>109</v>
       </c>
-      <c r="B33" s="212">
-        <v>1</v>
-      </c>
-      <c r="C33" s="213">
-        <v>1</v>
-      </c>
-      <c r="D33" s="215"/>
-      <c r="E33" s="213">
-        <v>1</v>
-      </c>
-      <c r="F33" s="216"/>
-      <c r="G33" s="213">
-        <v>1</v>
-      </c>
-      <c r="H33" s="197"/>
-      <c r="I33" s="178"/>
-      <c r="J33" s="300"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="183" t="s">
+      <c r="B33" s="206">
+        <v>1</v>
+      </c>
+      <c r="C33" s="207">
+        <v>1</v>
+      </c>
+      <c r="D33" s="209">
+        <v>1</v>
+      </c>
+      <c r="E33" s="207">
+        <v>1</v>
+      </c>
+      <c r="F33" s="210">
+        <v>0.75</v>
+      </c>
+      <c r="G33" s="207">
+        <v>1</v>
+      </c>
+      <c r="H33" s="176"/>
+      <c r="I33" s="176"/>
+      <c r="J33" s="286"/>
+      <c r="K33" s="286"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="181" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="179">
-        <v>1</v>
-      </c>
-      <c r="C34" s="199">
-        <v>1</v>
-      </c>
-      <c r="D34" s="203"/>
-      <c r="E34" s="199">
-        <v>1</v>
-      </c>
-      <c r="F34" s="217"/>
-      <c r="G34" s="199">
-        <v>1</v>
-      </c>
-      <c r="H34" s="197"/>
-      <c r="I34" s="178"/>
-      <c r="J34" s="300"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="202" t="s">
+      <c r="B34" s="177">
+        <v>1</v>
+      </c>
+      <c r="C34" s="194">
+        <v>1</v>
+      </c>
+      <c r="D34" s="198">
+        <v>1</v>
+      </c>
+      <c r="E34" s="194">
+        <v>1</v>
+      </c>
+      <c r="F34" s="211">
+        <v>1</v>
+      </c>
+      <c r="G34" s="194">
+        <v>1</v>
+      </c>
+      <c r="H34" s="176"/>
+      <c r="I34" s="176"/>
+      <c r="J34" s="286"/>
+      <c r="K34" s="286"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="197" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="179">
+      <c r="B35" s="177">
         <v>0.75</v>
       </c>
-      <c r="C35" s="199">
-        <v>3</v>
-      </c>
-      <c r="D35" s="203"/>
-      <c r="E35" s="199">
-        <v>3</v>
-      </c>
-      <c r="F35" s="214"/>
-      <c r="G35" s="199">
-        <v>3</v>
-      </c>
-      <c r="H35" s="197"/>
-      <c r="I35" s="178"/>
-      <c r="J35" s="300"/>
-    </row>
-    <row r="36" spans="1:10" ht="30">
-      <c r="A36" s="205" t="s">
+      <c r="C35" s="194">
+        <v>3</v>
+      </c>
+      <c r="D35" s="198">
+        <v>0.75</v>
+      </c>
+      <c r="E35" s="194">
+        <v>3</v>
+      </c>
+      <c r="F35" s="208">
+        <v>1</v>
+      </c>
+      <c r="G35" s="194">
+        <v>3</v>
+      </c>
+      <c r="H35" s="176"/>
+      <c r="I35" s="176"/>
+      <c r="J35" s="286"/>
+      <c r="K35" s="286"/>
+    </row>
+    <row r="36" spans="1:11" ht="30">
+      <c r="A36" s="200" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="179">
-        <v>1</v>
-      </c>
-      <c r="C36" s="180">
-        <v>3</v>
-      </c>
-      <c r="D36" s="203"/>
-      <c r="E36" s="180">
-        <v>3</v>
-      </c>
-      <c r="F36" s="214"/>
-      <c r="G36" s="180">
-        <v>3</v>
-      </c>
-      <c r="H36" s="178"/>
-      <c r="I36" s="178"/>
-      <c r="J36" s="300"/>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="208" t="s">
+      <c r="B36" s="177">
+        <v>1</v>
+      </c>
+      <c r="C36" s="178">
+        <v>3</v>
+      </c>
+      <c r="D36" s="198">
+        <v>1</v>
+      </c>
+      <c r="E36" s="178">
+        <v>3</v>
+      </c>
+      <c r="F36" s="208">
+        <v>1</v>
+      </c>
+      <c r="G36" s="178">
+        <v>3</v>
+      </c>
+      <c r="H36" s="176"/>
+      <c r="I36" s="176"/>
+      <c r="J36" s="286"/>
+      <c r="K36" s="286"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="218">
+      <c r="B37" s="212">
         <f>SUMPRODUCT(B33:B36,C33:C36)</f>
         <v>7.25</v>
       </c>
-      <c r="C37" s="188">
+      <c r="C37" s="186">
         <f>SUM(C33:C36)</f>
         <v>8</v>
       </c>
-      <c r="D37" s="219">
+      <c r="D37" s="213">
         <f>SUMPRODUCT(D33:D36,E33:E36)</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="190">
+        <v>7.25</v>
+      </c>
+      <c r="E37" s="188">
         <f>SUM(E33:E36)</f>
         <v>8</v>
       </c>
-      <c r="F37" s="191">
+      <c r="F37" s="189">
         <f>SUMPRODUCT(F33:F36,G33:G36)</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="192">
+        <v>7.75</v>
+      </c>
+      <c r="G37" s="190">
         <f>SUM(G33:G36)</f>
         <v>8</v>
       </c>
-      <c r="H37" s="197"/>
-      <c r="I37" s="178"/>
-      <c r="J37" s="300"/>
-    </row>
-    <row r="38" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A38" s="291" t="s">
+      <c r="H37" s="176"/>
+      <c r="I37" s="176"/>
+      <c r="J37" s="286"/>
+      <c r="K37" s="286"/>
+    </row>
+    <row r="38" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A38" s="282" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="291"/>
-      <c r="C38" s="291"/>
-      <c r="D38" s="291"/>
-      <c r="E38" s="291"/>
-      <c r="F38" s="291"/>
-      <c r="G38" s="291"/>
-      <c r="H38" s="162" t="s">
+      <c r="B38" s="282"/>
+      <c r="C38" s="282"/>
+      <c r="D38" s="282"/>
+      <c r="E38" s="282"/>
+      <c r="F38" s="282"/>
+      <c r="G38" s="282"/>
+      <c r="H38" s="160" t="s">
         <v>114</v>
       </c>
-      <c r="I38" s="162"/>
-      <c r="J38" s="300"/>
-    </row>
-    <row r="39" spans="1:10" ht="45">
-      <c r="A39" s="202" t="s">
+      <c r="I38" s="160"/>
+      <c r="J38" s="286"/>
+      <c r="K38" s="286"/>
+    </row>
+    <row r="39" spans="1:11" ht="45">
+      <c r="A39" s="197" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="212">
-        <v>1</v>
-      </c>
-      <c r="C39" s="194">
-        <v>1</v>
-      </c>
-      <c r="D39" s="203"/>
-      <c r="E39" s="194">
-        <v>1</v>
-      </c>
-      <c r="F39" s="214"/>
-      <c r="G39" s="194">
-        <v>1</v>
-      </c>
-      <c r="H39" s="178"/>
-      <c r="I39" s="178"/>
-      <c r="J39" s="300"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="202" t="s">
+      <c r="B39" s="206">
+        <v>1</v>
+      </c>
+      <c r="C39" s="191">
+        <v>1</v>
+      </c>
+      <c r="D39" s="198">
+        <v>0.5</v>
+      </c>
+      <c r="E39" s="191">
+        <v>1</v>
+      </c>
+      <c r="F39" s="208">
+        <v>1</v>
+      </c>
+      <c r="G39" s="191">
+        <v>1</v>
+      </c>
+      <c r="H39" s="176"/>
+      <c r="I39" s="176"/>
+      <c r="J39" s="286"/>
+      <c r="K39" s="286"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="179">
-        <v>1</v>
-      </c>
-      <c r="C40" s="199">
+      <c r="B40" s="177">
+        <v>1</v>
+      </c>
+      <c r="C40" s="194">
         <v>4</v>
       </c>
-      <c r="D40" s="203"/>
-      <c r="E40" s="199">
+      <c r="D40" s="198">
+        <v>0.25</v>
+      </c>
+      <c r="E40" s="194">
         <v>4</v>
       </c>
-      <c r="F40" s="214"/>
-      <c r="G40" s="199">
+      <c r="F40" s="208">
+        <v>1</v>
+      </c>
+      <c r="G40" s="194">
         <v>4</v>
       </c>
-      <c r="H40" s="178"/>
-      <c r="I40" s="178"/>
-      <c r="J40" s="300"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="202" t="s">
+      <c r="H40" s="176"/>
+      <c r="I40" s="176"/>
+      <c r="J40" s="286"/>
+      <c r="K40" s="286"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="197" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="179">
-        <v>1</v>
-      </c>
-      <c r="C41" s="199">
-        <v>3</v>
-      </c>
-      <c r="D41" s="203"/>
-      <c r="E41" s="199">
-        <v>3</v>
-      </c>
-      <c r="F41" s="214"/>
-      <c r="G41" s="199">
-        <v>3</v>
-      </c>
-      <c r="H41" s="178"/>
-      <c r="I41" s="178"/>
-      <c r="J41" s="300"/>
-    </row>
-    <row r="42" spans="1:10" ht="60">
-      <c r="A42" s="202" t="s">
+      <c r="B41" s="177">
+        <v>1</v>
+      </c>
+      <c r="C41" s="194">
+        <v>3</v>
+      </c>
+      <c r="D41" s="198">
+        <v>0.5</v>
+      </c>
+      <c r="E41" s="194">
+        <v>3</v>
+      </c>
+      <c r="F41" s="208">
+        <v>0.25</v>
+      </c>
+      <c r="G41" s="194">
+        <v>3</v>
+      </c>
+      <c r="H41" s="176"/>
+      <c r="I41" s="176"/>
+      <c r="J41" s="286"/>
+      <c r="K41" s="286"/>
+    </row>
+    <row r="42" spans="1:11" ht="60">
+      <c r="A42" s="197" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="179">
+      <c r="B42" s="177">
         <v>0.5</v>
       </c>
-      <c r="C42" s="199">
+      <c r="C42" s="194">
         <v>2</v>
       </c>
-      <c r="D42" s="203"/>
-      <c r="E42" s="199">
+      <c r="D42" s="198">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="194">
         <v>2</v>
       </c>
-      <c r="F42" s="214"/>
-      <c r="G42" s="199">
+      <c r="F42" s="208">
+        <v>1</v>
+      </c>
+      <c r="G42" s="194">
         <v>2</v>
       </c>
-      <c r="H42" s="178"/>
-      <c r="J42" s="300"/>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="202" t="s">
+      <c r="H42" s="176"/>
+      <c r="J42" s="286"/>
+      <c r="K42" s="286"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="197" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="179">
+      <c r="B43" s="177">
         <v>0.5</v>
       </c>
-      <c r="C43" s="199">
+      <c r="C43" s="194">
         <v>2</v>
       </c>
-      <c r="D43" s="203"/>
-      <c r="E43" s="199">
+      <c r="D43" s="198">
+        <v>0.25</v>
+      </c>
+      <c r="E43" s="194">
         <v>2</v>
       </c>
-      <c r="F43" s="214"/>
-      <c r="G43" s="199">
+      <c r="F43" s="208">
+        <v>1</v>
+      </c>
+      <c r="G43" s="194">
         <v>2</v>
       </c>
-      <c r="H43" s="178"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="300"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="202" t="s">
+      <c r="H43" s="176"/>
+      <c r="I43" s="176"/>
+      <c r="J43" s="286"/>
+      <c r="K43" s="286"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="197" t="s">
         <v>120</v>
       </c>
-      <c r="B44" s="179">
-        <v>1</v>
-      </c>
-      <c r="C44" s="199">
-        <v>3</v>
-      </c>
-      <c r="D44" s="203"/>
-      <c r="E44" s="199">
-        <v>3</v>
-      </c>
-      <c r="F44" s="214"/>
-      <c r="G44" s="199">
-        <v>3</v>
-      </c>
-      <c r="H44" s="178"/>
-      <c r="I44" s="178"/>
-      <c r="J44" s="300"/>
-    </row>
-    <row r="45" spans="1:10" ht="30">
-      <c r="A45" s="202" t="s">
+      <c r="B44" s="177">
+        <v>1</v>
+      </c>
+      <c r="C44" s="194">
+        <v>3</v>
+      </c>
+      <c r="D44" s="198">
+        <v>1</v>
+      </c>
+      <c r="E44" s="194">
+        <v>3</v>
+      </c>
+      <c r="F44" s="208">
+        <v>1</v>
+      </c>
+      <c r="G44" s="194">
+        <v>3</v>
+      </c>
+      <c r="H44" s="176"/>
+      <c r="I44" s="176"/>
+      <c r="J44" s="286"/>
+      <c r="K44" s="286"/>
+    </row>
+    <row r="45" spans="1:11" ht="30">
+      <c r="A45" s="197" t="s">
         <v>121</v>
       </c>
-      <c r="B45" s="179">
+      <c r="B45" s="177">
         <v>0.75</v>
       </c>
-      <c r="C45" s="199">
-        <v>3</v>
-      </c>
-      <c r="D45" s="203"/>
-      <c r="E45" s="199">
-        <v>3</v>
-      </c>
-      <c r="F45" s="214"/>
-      <c r="G45" s="199">
-        <v>3</v>
-      </c>
-      <c r="H45" s="178"/>
-      <c r="I45" s="178"/>
-      <c r="J45" s="300"/>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="202" t="s">
+      <c r="C45" s="194">
+        <v>3</v>
+      </c>
+      <c r="D45" s="198">
+        <v>0.5</v>
+      </c>
+      <c r="E45" s="194">
+        <v>3</v>
+      </c>
+      <c r="F45" s="208">
+        <v>0.5</v>
+      </c>
+      <c r="G45" s="194">
+        <v>3</v>
+      </c>
+      <c r="H45" s="176"/>
+      <c r="I45" s="176"/>
+      <c r="J45" s="286"/>
+      <c r="K45" s="286"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="197" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="179">
+      <c r="B46" s="177">
         <v>0.5</v>
       </c>
-      <c r="C46" s="199">
+      <c r="C46" s="194">
         <v>4</v>
       </c>
-      <c r="D46" s="203"/>
-      <c r="E46" s="199">
+      <c r="D46" s="198">
+        <v>1</v>
+      </c>
+      <c r="E46" s="194">
         <v>4</v>
       </c>
-      <c r="F46" s="214"/>
-      <c r="G46" s="199">
+      <c r="F46" s="208">
+        <v>1</v>
+      </c>
+      <c r="G46" s="194">
         <v>4</v>
       </c>
-      <c r="H46" s="178"/>
-      <c r="I46" s="178"/>
-      <c r="J46" s="300"/>
-    </row>
-    <row r="47" spans="1:10" ht="60">
-      <c r="A47" s="205" t="s">
+      <c r="H46" s="176"/>
+      <c r="I46" s="176"/>
+      <c r="J46" s="286"/>
+      <c r="K46" s="286"/>
+    </row>
+    <row r="47" spans="1:11" ht="60">
+      <c r="A47" s="200" t="s">
         <v>123</v>
       </c>
-      <c r="B47" s="179">
-        <v>1</v>
-      </c>
-      <c r="C47" s="180">
+      <c r="B47" s="177">
+        <v>1</v>
+      </c>
+      <c r="C47" s="178">
         <v>10</v>
       </c>
-      <c r="D47" s="203"/>
-      <c r="E47" s="180">
+      <c r="D47" s="198">
+        <v>0.25</v>
+      </c>
+      <c r="E47" s="178">
         <v>10</v>
       </c>
-      <c r="F47" s="214"/>
-      <c r="G47" s="180">
+      <c r="F47" s="208">
+        <v>0.75</v>
+      </c>
+      <c r="G47" s="178">
         <v>10</v>
       </c>
-      <c r="H47" s="178"/>
-      <c r="I47" s="178"/>
-      <c r="J47" s="300"/>
-    </row>
-    <row r="48" spans="1:10" ht="30">
-      <c r="A48" s="205" t="s">
+      <c r="H47" s="176"/>
+      <c r="I47" s="176"/>
+      <c r="J47" s="286"/>
+      <c r="K47" s="286"/>
+    </row>
+    <row r="48" spans="1:11" ht="30">
+      <c r="A48" s="200" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="179">
+      <c r="B48" s="177">
         <v>0.75</v>
       </c>
-      <c r="C48" s="180">
+      <c r="C48" s="178">
         <v>6</v>
       </c>
-      <c r="D48" s="203"/>
-      <c r="E48" s="180">
+      <c r="D48" s="198">
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="178">
         <v>6</v>
       </c>
-      <c r="F48" s="214"/>
-      <c r="G48" s="180">
+      <c r="F48" s="208">
+        <v>0.5</v>
+      </c>
+      <c r="G48" s="178">
         <v>6</v>
       </c>
-      <c r="H48" s="178"/>
-      <c r="I48" s="178"/>
-      <c r="J48" s="300"/>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="205" t="s">
+      <c r="H48" s="176"/>
+      <c r="I48" s="176"/>
+      <c r="J48" s="286"/>
+      <c r="K48" s="286"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="200" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="179">
-        <v>1</v>
-      </c>
-      <c r="C49" s="180">
-        <v>3</v>
-      </c>
-      <c r="D49" s="203"/>
-      <c r="E49" s="180">
-        <v>3</v>
-      </c>
-      <c r="F49" s="214"/>
-      <c r="G49" s="180">
-        <v>3</v>
-      </c>
-      <c r="H49" s="178"/>
-      <c r="I49" s="178"/>
-      <c r="J49" s="300"/>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="208" t="s">
+      <c r="B49" s="177">
+        <v>1</v>
+      </c>
+      <c r="C49" s="178">
+        <v>3</v>
+      </c>
+      <c r="D49" s="198">
+        <v>1</v>
+      </c>
+      <c r="E49" s="178">
+        <v>3</v>
+      </c>
+      <c r="F49" s="208">
+        <v>1</v>
+      </c>
+      <c r="G49" s="178">
+        <v>3</v>
+      </c>
+      <c r="H49" s="176"/>
+      <c r="I49" s="176"/>
+      <c r="J49" s="286"/>
+      <c r="K49" s="286"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="203" t="s">
         <v>91</v>
       </c>
-      <c r="B50" s="218">
+      <c r="B50" s="212">
         <f>SUMPRODUCT(B39:B49,C39:C49)</f>
         <v>34.75</v>
       </c>
-      <c r="C50" s="188">
+      <c r="C50" s="186">
         <f>SUM(C39:C49)</f>
         <v>41</v>
       </c>
-      <c r="D50" s="219">
+      <c r="D50" s="213">
         <f>SUMPRODUCT(D39:D49,E39:E49)</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="190">
+        <v>21.5</v>
+      </c>
+      <c r="E50" s="188">
         <f>SUM(E39:E49)</f>
         <v>41</v>
       </c>
-      <c r="F50" s="191">
+      <c r="F50" s="189">
         <f>SUMPRODUCT(F39:F49,G39:G49)</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="192">
+        <v>31.75</v>
+      </c>
+      <c r="G50" s="190">
         <f>SUM(G39:G49)</f>
         <v>41</v>
       </c>
-      <c r="H50" s="197"/>
-      <c r="I50" s="178"/>
-      <c r="J50" s="300"/>
-    </row>
-    <row r="51" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A51" s="291" t="s">
+      <c r="H50" s="176"/>
+      <c r="I50" s="176"/>
+      <c r="J50" s="286"/>
+      <c r="K50" s="286"/>
+    </row>
+    <row r="51" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A51" s="282" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="291"/>
-      <c r="C51" s="291"/>
-      <c r="D51" s="291"/>
-      <c r="E51" s="291"/>
-      <c r="F51" s="291"/>
-      <c r="G51" s="291"/>
-      <c r="H51" s="162" t="s">
+      <c r="B51" s="282"/>
+      <c r="C51" s="282"/>
+      <c r="D51" s="282"/>
+      <c r="E51" s="282"/>
+      <c r="F51" s="282"/>
+      <c r="G51" s="282"/>
+      <c r="H51" s="160" t="s">
         <v>103</v>
       </c>
-      <c r="I51" s="162"/>
-      <c r="J51" s="300"/>
-    </row>
-    <row r="52" spans="1:10" ht="30">
-      <c r="A52" s="220" t="s">
+      <c r="I51" s="160"/>
+      <c r="J51" s="286"/>
+      <c r="K51" s="286"/>
+    </row>
+    <row r="52" spans="1:11" ht="30">
+      <c r="A52" s="214" t="s">
         <v>127</v>
       </c>
-      <c r="B52" s="212">
-        <v>1</v>
-      </c>
-      <c r="C52" s="221">
+      <c r="B52" s="206">
+        <v>1</v>
+      </c>
+      <c r="C52" s="215">
         <v>2</v>
       </c>
-      <c r="D52" s="222"/>
-      <c r="E52" s="221">
+      <c r="D52" s="216">
+        <v>1</v>
+      </c>
+      <c r="E52" s="215">
         <v>2</v>
       </c>
-      <c r="F52" s="216"/>
-      <c r="G52" s="221">
+      <c r="F52" s="210">
+        <v>1</v>
+      </c>
+      <c r="G52" s="215">
         <v>2</v>
       </c>
-      <c r="H52" s="197"/>
-      <c r="I52" s="178"/>
-      <c r="J52" s="300"/>
-    </row>
-    <row r="53" spans="1:10" ht="30">
-      <c r="A53" s="185" t="s">
+      <c r="H52" s="176"/>
+      <c r="I52" s="176"/>
+      <c r="J52" s="286"/>
+      <c r="K52" s="286"/>
+    </row>
+    <row r="53" spans="1:11" ht="30">
+      <c r="A53" s="183" t="s">
         <v>128</v>
       </c>
-      <c r="B53" s="223">
-        <v>1</v>
-      </c>
-      <c r="C53" s="180">
+      <c r="B53" s="217">
+        <v>1</v>
+      </c>
+      <c r="C53" s="178">
         <v>2</v>
       </c>
-      <c r="D53" s="224"/>
-      <c r="E53" s="180">
+      <c r="D53" s="218">
+        <v>1</v>
+      </c>
+      <c r="E53" s="178">
         <v>2</v>
       </c>
-      <c r="F53" s="214"/>
-      <c r="G53" s="180">
+      <c r="F53" s="208">
+        <v>1</v>
+      </c>
+      <c r="G53" s="178">
         <v>2</v>
       </c>
-      <c r="H53" s="178"/>
-      <c r="I53" s="178"/>
-      <c r="J53" s="300"/>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="185" t="s">
+      <c r="H53" s="176"/>
+      <c r="I53" s="176"/>
+      <c r="J53" s="286"/>
+      <c r="K53" s="286"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="183" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="225">
-        <v>1</v>
-      </c>
-      <c r="C54" s="180">
-        <v>1</v>
-      </c>
-      <c r="D54" s="203"/>
-      <c r="E54" s="180">
-        <v>1</v>
-      </c>
-      <c r="F54" s="217"/>
-      <c r="G54" s="180">
-        <v>1</v>
-      </c>
-      <c r="H54" s="178"/>
-      <c r="I54" s="178"/>
-      <c r="J54" s="300"/>
-    </row>
-    <row r="55" spans="1:10" ht="120" customHeight="1">
-      <c r="A55" s="185" t="s">
+      <c r="B54" s="219">
+        <v>1</v>
+      </c>
+      <c r="C54" s="178">
+        <v>1</v>
+      </c>
+      <c r="D54" s="198">
+        <v>1</v>
+      </c>
+      <c r="E54" s="178">
+        <v>1</v>
+      </c>
+      <c r="F54" s="211">
+        <v>1</v>
+      </c>
+      <c r="G54" s="178">
+        <v>1</v>
+      </c>
+      <c r="H54" s="176"/>
+      <c r="I54" s="176"/>
+      <c r="J54" s="286"/>
+      <c r="K54" s="286"/>
+    </row>
+    <row r="55" spans="1:11" ht="120" customHeight="1">
+      <c r="A55" s="183" t="s">
         <v>130</v>
       </c>
-      <c r="B55" s="225">
-        <v>1</v>
-      </c>
-      <c r="C55" s="180">
+      <c r="B55" s="219">
+        <v>1</v>
+      </c>
+      <c r="C55" s="178">
         <v>4</v>
       </c>
-      <c r="D55" s="203"/>
-      <c r="E55" s="180">
+      <c r="D55" s="198">
+        <v>1</v>
+      </c>
+      <c r="E55" s="178">
         <v>4</v>
       </c>
-      <c r="F55" s="217"/>
-      <c r="G55" s="180">
+      <c r="F55" s="211">
+        <v>1</v>
+      </c>
+      <c r="G55" s="178">
         <v>4</v>
       </c>
-      <c r="H55" s="178"/>
-      <c r="I55" s="178"/>
-      <c r="J55" s="300"/>
-    </row>
-    <row r="56" spans="1:10" ht="45">
-      <c r="A56" s="184" t="s">
+      <c r="H55" s="176"/>
+      <c r="I55" s="176"/>
+      <c r="J55" s="286"/>
+      <c r="K55" s="286"/>
+    </row>
+    <row r="56" spans="1:11" ht="45">
+      <c r="A56" s="182" t="s">
         <v>131</v>
       </c>
-      <c r="B56" s="281">
-        <v>1</v>
-      </c>
-      <c r="C56" s="199">
+      <c r="B56" s="201">
+        <v>1</v>
+      </c>
+      <c r="C56" s="194">
         <v>2</v>
       </c>
-      <c r="D56" s="280"/>
-      <c r="E56" s="199">
+      <c r="D56" s="274">
+        <v>1</v>
+      </c>
+      <c r="E56" s="194">
         <v>2</v>
       </c>
-      <c r="F56" s="282"/>
-      <c r="G56" s="199">
+      <c r="F56" s="275">
+        <v>1</v>
+      </c>
+      <c r="G56" s="194">
         <v>2</v>
       </c>
-      <c r="H56" s="226"/>
-      <c r="I56" s="178"/>
-      <c r="J56" s="300"/>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="227" t="s">
+      <c r="H56" s="220"/>
+      <c r="I56" s="176"/>
+      <c r="J56" s="286"/>
+      <c r="K56" s="286"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="221" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="187">
+      <c r="B57" s="185">
         <f>SUMPRODUCT(B52:B56,C52:C56)</f>
         <v>11</v>
       </c>
-      <c r="C57" s="188">
+      <c r="C57" s="186">
         <f>SUM(C52:C56)</f>
         <v>11</v>
       </c>
-      <c r="D57" s="189">
+      <c r="D57" s="187">
         <f>SUMPRODUCT(D52:D56,E52:E56)</f>
-        <v>0</v>
-      </c>
-      <c r="E57" s="190">
+        <v>11</v>
+      </c>
+      <c r="E57" s="188">
         <f>SUM(E52:E56)</f>
         <v>11</v>
       </c>
-      <c r="F57" s="228">
+      <c r="F57" s="222">
         <f>SUMPRODUCT(F52:F56,G52:G56)</f>
-        <v>0</v>
-      </c>
-      <c r="G57" s="229">
+        <v>11</v>
+      </c>
+      <c r="G57" s="223">
         <f>SUM(G52:G56)</f>
         <v>11</v>
       </c>
-      <c r="H57" s="178"/>
-      <c r="I57" s="178"/>
-    </row>
-    <row r="58" spans="1:10" ht="18.399999999999999" customHeight="1">
-      <c r="A58" s="291" t="s">
+      <c r="H57" s="176"/>
+      <c r="I57" s="176"/>
+    </row>
+    <row r="58" spans="1:11" ht="18.399999999999999" customHeight="1">
+      <c r="A58" s="282" t="s">
         <v>76</v>
       </c>
-      <c r="B58" s="291"/>
-      <c r="C58" s="291"/>
-      <c r="D58" s="291"/>
-      <c r="E58" s="291"/>
-      <c r="F58" s="291"/>
-      <c r="G58" s="291"/>
-      <c r="H58" s="162"/>
-      <c r="I58" s="162"/>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="230" t="s">
+      <c r="B58" s="282"/>
+      <c r="C58" s="282"/>
+      <c r="D58" s="282"/>
+      <c r="E58" s="282"/>
+      <c r="F58" s="282"/>
+      <c r="G58" s="282"/>
+      <c r="H58" s="160"/>
+      <c r="I58" s="160"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="224" t="s">
         <v>132</v>
       </c>
-      <c r="B59" s="231">
+      <c r="B59" s="225">
         <f t="shared" ref="B59:G59" si="0">B13+B20+B25+B31+B37+B50+B57</f>
         <v>82</v>
       </c>
-      <c r="C59" s="194">
+      <c r="C59" s="191">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="D59" s="232">
+      <c r="D59" s="226">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E59" s="233">
+        <v>71</v>
+      </c>
+      <c r="E59" s="227">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F59" s="234">
+      <c r="F59" s="228">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G59" s="235">
+        <v>86.5</v>
+      </c>
+      <c r="G59" s="229">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H59" s="226"/>
-      <c r="I59" s="178"/>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="230" t="s">
+      <c r="H59" s="220"/>
+      <c r="I59" s="176"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="296">
+      <c r="B60" s="283">
         <f>B59/C59</f>
         <v>0.82</v>
       </c>
-      <c r="C60" s="296"/>
-      <c r="D60" s="297">
+      <c r="C60" s="283"/>
+      <c r="D60" s="284">
         <f>D59/E59</f>
-        <v>0</v>
-      </c>
-      <c r="E60" s="297"/>
-      <c r="F60" s="298">
+        <v>0.71</v>
+      </c>
+      <c r="E60" s="284"/>
+      <c r="F60" s="285">
         <f>F59/G59</f>
-        <v>0</v>
-      </c>
-      <c r="G60" s="298"/>
-      <c r="H60" s="236"/>
-      <c r="I60" s="236"/>
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="G60" s="285"/>
+      <c r="H60" s="230"/>
+      <c r="I60" s="230"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="D60:E60"/>
@@ -6991,12 +7140,7 @@
     <mergeCell ref="A32:G32"/>
     <mergeCell ref="A38:G38"/>
     <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="K7:K56"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13 H20 H25 H31 H37 H50" xr:uid="{00000000-0002-0000-0600-000000000000}">
@@ -7048,7 +7192,7 @@
       <c r="F2" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="288" t="s">
+      <c r="G2" s="280" t="s">
         <v>3</v>
       </c>
     </row>
@@ -7061,7 +7205,7 @@
       <c r="D3" s="55"/>
       <c r="E3" s="56"/>
       <c r="F3" s="57"/>
-      <c r="G3" s="288"/>
+      <c r="G3" s="280"/>
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="58" t="s">
@@ -7399,7 +7543,6 @@
         <f>SUMPRODUCT(F$4:F$27,$G$4:$G$27)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="161"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="85" t="s">
@@ -7425,7 +7568,6 @@
         <f>SUMPRODUCT(--ISNUMBER(F$4:F$27),$G$4:$G$27)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="161"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="91" t="s">
@@ -7456,15 +7598,10 @@
       <c r="A33" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="161"/>
-      <c r="C33" s="161"/>
-      <c r="D33" s="161"/>
-      <c r="E33" s="161"/>
-      <c r="F33" s="161"/>
-      <c r="H33" s="289" t="s">
+      <c r="H33" s="281" t="s">
         <v>55</v>
       </c>
-      <c r="I33" s="289"/>
+      <c r="I33" s="281"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="52" t="s">
@@ -7667,24 +7804,16 @@
         <f>IF(F$34="Oui",$H$43,$I$43)</f>
         <v>10</v>
       </c>
-      <c r="H44" s="136"/>
-      <c r="I44" s="136"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="137"/>
-      <c r="B45" s="137"/>
-      <c r="C45" s="137"/>
-      <c r="D45" s="137"/>
-      <c r="E45" s="137"/>
-      <c r="F45" s="137"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="161"/>
-      <c r="B46" s="161"/>
-      <c r="C46" s="161"/>
-      <c r="D46" s="161"/>
-      <c r="E46" s="161"/>
-      <c r="F46" s="161"/>
+      <c r="A45" s="136"/>
+      <c r="B45" s="136"/>
+      <c r="C45" s="136"/>
+      <c r="D45" s="136"/>
+      <c r="E45" s="136"/>
+      <c r="F45" s="136"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="91" t="s">
@@ -7715,7 +7844,7 @@
       <c r="A50" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="B50" s="138">
+      <c r="B50" s="137">
         <f>(B$31+B$47)/2</f>
         <v>0.5</v>
       </c>
@@ -7740,23 +7869,23 @@
       <c r="A51" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="B51" s="139">
+      <c r="B51" s="138">
         <f>COUNTA(B$4:B$27)</f>
         <v>0</v>
       </c>
-      <c r="C51" s="140">
+      <c r="C51" s="139">
         <f>COUNTA(C$4:C$27)</f>
         <v>0</v>
       </c>
-      <c r="D51" s="141">
+      <c r="D51" s="140">
         <f>COUNTA(D$4:D$27)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="142">
+      <c r="E51" s="141">
         <f>COUNTA(E$4:E$27)</f>
         <v>0</v>
       </c>
-      <c r="F51" s="143">
+      <c r="F51" s="142">
         <f>COUNTA(F$4:F$27)</f>
         <v>0</v>
       </c>
@@ -7786,8 +7915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7802,825 +7931,986 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="301" t="s">
+      <c r="A1" s="296" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
+      <c r="B1" s="296"/>
+      <c r="C1" s="296"/>
+      <c r="D1" s="296"/>
+      <c r="E1" s="296"/>
+      <c r="F1" s="296"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="283"/>
-      <c r="B2" s="283"/>
-      <c r="C2" s="237"/>
-      <c r="D2" s="237"/>
-      <c r="E2" s="283"/>
-      <c r="F2" s="237"/>
+      <c r="A2" s="170"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="231"/>
     </row>
     <row r="3" spans="1:8" ht="18.75">
-      <c r="A3" s="301" t="s">
+      <c r="A3" s="296" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="301"/>
-      <c r="C3" s="301"/>
-      <c r="D3" s="301"/>
-      <c r="E3" s="301"/>
-      <c r="F3" s="301"/>
+      <c r="B3" s="296"/>
+      <c r="C3" s="296"/>
+      <c r="D3" s="296"/>
+      <c r="E3" s="296"/>
+      <c r="F3" s="296"/>
     </row>
     <row r="5" spans="1:8" ht="23.25">
-      <c r="A5" s="302" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="302"/>
-      <c r="C5" s="302"/>
-      <c r="D5" s="302"/>
-      <c r="E5" s="302"/>
-      <c r="F5" s="302"/>
+      <c r="A5" s="297" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="297"/>
+      <c r="C5" s="297"/>
+      <c r="D5" s="297"/>
+      <c r="E5" s="297"/>
+      <c r="F5" s="297"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="238" t="s">
+      <c r="A6" s="232" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="303"/>
-      <c r="C6" s="303"/>
-      <c r="D6" s="303"/>
-      <c r="E6" s="303"/>
-      <c r="F6" s="303"/>
+      <c r="B6" s="298"/>
+      <c r="C6" s="298"/>
+      <c r="D6" s="298"/>
+      <c r="E6" s="298"/>
+      <c r="F6" s="298"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="239" t="s">
+      <c r="A7" s="233" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="240" t="s">
+      <c r="B7" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="240" t="s">
+      <c r="C7" s="234" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="240" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="240" t="s">
+      <c r="D7" s="234" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="234" t="s">
         <v>160</v>
       </c>
-      <c r="F7" s="241" t="s">
+      <c r="F7" s="235" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="242" t="s">
+      <c r="A8" s="236" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="243">
-        <v>1</v>
-      </c>
-      <c r="C8" s="243">
+      <c r="B8" s="237">
+        <v>1</v>
+      </c>
+      <c r="C8" s="237">
         <v>0.75</v>
       </c>
-      <c r="D8" s="243">
+      <c r="D8" s="237">
         <v>16</v>
       </c>
-      <c r="E8" s="243">
+      <c r="E8" s="237">
         <f t="shared" ref="E8:E17" si="0">B8*C8*D8</f>
         <v>12</v>
       </c>
-      <c r="F8" s="244"/>
+      <c r="F8" s="238"/>
       <c r="G8" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="300" t="s">
+      <c r="H8" s="286" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="242" t="s">
+      <c r="A9" s="236" t="s">
         <v>162</v>
       </c>
-      <c r="B9" s="243">
-        <v>1</v>
-      </c>
-      <c r="C9" s="243">
-        <v>1</v>
-      </c>
-      <c r="D9" s="243">
+      <c r="B9" s="237">
+        <v>1</v>
+      </c>
+      <c r="C9" s="237">
+        <v>1</v>
+      </c>
+      <c r="D9" s="237">
         <v>8</v>
       </c>
-      <c r="E9" s="243">
+      <c r="E9" s="237">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F9" s="245"/>
+      <c r="F9" s="239"/>
       <c r="G9" t="s">
         <v>84</v>
       </c>
-      <c r="H9" s="300"/>
+      <c r="H9" s="286"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="242" t="s">
+      <c r="A10" s="236" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="243">
-        <v>1</v>
-      </c>
-      <c r="C10" s="243">
-        <v>1</v>
-      </c>
-      <c r="D10" s="243">
+      <c r="B10" s="237">
+        <v>1</v>
+      </c>
+      <c r="C10" s="237">
+        <v>1</v>
+      </c>
+      <c r="D10" s="237">
         <v>14</v>
       </c>
-      <c r="E10" s="243">
+      <c r="E10" s="237">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="F10" s="245"/>
+      <c r="F10" s="239"/>
       <c r="G10" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="300"/>
+      <c r="H10" s="286"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="242" t="s">
+      <c r="A11" s="236" t="s">
         <v>164</v>
       </c>
-      <c r="B11" s="243">
-        <v>1</v>
-      </c>
-      <c r="C11" s="243">
-        <v>1</v>
-      </c>
-      <c r="D11" s="243">
+      <c r="B11" s="237">
+        <v>1</v>
+      </c>
+      <c r="C11" s="237">
+        <v>1</v>
+      </c>
+      <c r="D11" s="237">
         <v>12</v>
       </c>
-      <c r="E11" s="243">
+      <c r="E11" s="237">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F11" s="245"/>
+      <c r="F11" s="239"/>
       <c r="G11" t="s">
         <v>84</v>
       </c>
-      <c r="H11" s="300"/>
+      <c r="H11" s="286"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="242" t="s">
+      <c r="A12" s="236" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="243">
-        <v>1</v>
-      </c>
-      <c r="C12" s="243">
-        <v>1</v>
-      </c>
-      <c r="D12" s="243">
+      <c r="B12" s="237">
+        <v>1</v>
+      </c>
+      <c r="C12" s="237">
+        <v>1</v>
+      </c>
+      <c r="D12" s="237">
         <v>8</v>
       </c>
-      <c r="E12" s="243">
+      <c r="E12" s="237">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F12" s="244"/>
+      <c r="F12" s="238"/>
       <c r="G12" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="300"/>
+      <c r="H12" s="286"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="242" t="s">
+      <c r="A13" s="236" t="s">
         <v>166</v>
       </c>
-      <c r="B13" s="243">
-        <v>1</v>
-      </c>
-      <c r="C13" s="243">
-        <v>1</v>
-      </c>
-      <c r="D13" s="243">
+      <c r="B13" s="237">
+        <v>1</v>
+      </c>
+      <c r="C13" s="237">
+        <v>1</v>
+      </c>
+      <c r="D13" s="237">
         <v>10</v>
       </c>
-      <c r="E13" s="243">
+      <c r="E13" s="237">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F13" s="244"/>
+      <c r="F13" s="238"/>
       <c r="G13" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="300"/>
+      <c r="H13" s="286"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="242" t="s">
+      <c r="A14" s="236" t="s">
         <v>167</v>
       </c>
-      <c r="B14" s="243">
-        <v>1</v>
-      </c>
-      <c r="C14" s="243">
-        <v>1</v>
-      </c>
-      <c r="D14" s="243">
+      <c r="B14" s="237">
+        <v>1</v>
+      </c>
+      <c r="C14" s="237">
+        <v>1</v>
+      </c>
+      <c r="D14" s="237">
         <v>10</v>
       </c>
-      <c r="E14" s="243">
+      <c r="E14" s="237">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F14" s="244"/>
+      <c r="F14" s="238"/>
       <c r="G14" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="300"/>
+      <c r="H14" s="286"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="242" t="s">
+      <c r="A15" s="236" t="s">
         <v>168</v>
       </c>
-      <c r="B15" s="243">
+      <c r="B15" s="237">
         <v>0.93</v>
       </c>
-      <c r="C15" s="243">
-        <v>1</v>
-      </c>
-      <c r="D15" s="243">
+      <c r="C15" s="237">
+        <v>1</v>
+      </c>
+      <c r="D15" s="237">
         <v>8</v>
       </c>
-      <c r="E15" s="243">
+      <c r="E15" s="237">
         <f t="shared" si="0"/>
         <v>7.44</v>
       </c>
-      <c r="F15" s="244"/>
+      <c r="F15" s="238"/>
       <c r="G15" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="300"/>
+      <c r="H15" s="286"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="242" t="s">
+      <c r="A16" s="236" t="s">
         <v>169</v>
       </c>
-      <c r="B16" s="243">
+      <c r="B16" s="237">
         <v>0.93</v>
       </c>
-      <c r="C16" s="243">
-        <v>1</v>
-      </c>
-      <c r="D16" s="243">
+      <c r="C16" s="237">
+        <v>1</v>
+      </c>
+      <c r="D16" s="237">
         <v>8</v>
       </c>
-      <c r="E16" s="243">
+      <c r="E16" s="237">
         <f t="shared" si="0"/>
         <v>7.44</v>
       </c>
-      <c r="F16" s="244"/>
+      <c r="F16" s="238"/>
       <c r="G16" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="300"/>
+      <c r="H16" s="286"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="242" t="s">
+      <c r="A17" s="236" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="243">
-        <v>1</v>
-      </c>
-      <c r="C17" s="243">
-        <v>1</v>
-      </c>
-      <c r="D17" s="243">
+      <c r="B17" s="237">
+        <v>1</v>
+      </c>
+      <c r="C17" s="237">
+        <v>1</v>
+      </c>
+      <c r="D17" s="237">
         <v>6</v>
       </c>
-      <c r="E17" s="243">
+      <c r="E17" s="237">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F17" s="245"/>
+      <c r="F17" s="239"/>
       <c r="G17" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="300"/>
+      <c r="H17" s="286"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="246" t="s">
+      <c r="A18" s="240" t="s">
         <v>171</v>
       </c>
-      <c r="B18" s="304"/>
-      <c r="C18" s="304"/>
-      <c r="D18" s="284">
+      <c r="B18" s="299"/>
+      <c r="C18" s="299"/>
+      <c r="D18" s="276">
         <f>SUM(D8:D17)</f>
         <v>100</v>
       </c>
-      <c r="E18" s="247">
+      <c r="E18" s="241">
         <f>SUM(E8:E17)/D18 - E20*D20 - E19*D19</f>
         <v>0.94879999999999998</v>
       </c>
-      <c r="F18" s="248"/>
+      <c r="F18" s="242"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="249" t="s">
+      <c r="A19" s="243" t="s">
         <v>172</v>
       </c>
-      <c r="D19" s="250">
+      <c r="D19" s="244">
         <v>0.15</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="249" t="s">
+      <c r="A20" s="243" t="s">
         <v>173</v>
       </c>
-      <c r="D20" s="250">
+      <c r="D20" s="244">
         <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="23.25" customHeight="1">
-      <c r="A21" s="305" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="305"/>
-      <c r="C21" s="305"/>
-      <c r="D21" s="305"/>
-      <c r="E21" s="305"/>
-      <c r="F21" s="305"/>
+      <c r="A21" s="292" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="292"/>
+      <c r="C21" s="292"/>
+      <c r="D21" s="292"/>
+      <c r="E21" s="292"/>
+      <c r="F21" s="292"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="251" t="s">
+      <c r="A22" s="245" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="306"/>
-      <c r="C22" s="306"/>
-      <c r="D22" s="306"/>
-      <c r="E22" s="306"/>
-      <c r="F22" s="306"/>
+      <c r="B22" s="293"/>
+      <c r="C22" s="293"/>
+      <c r="D22" s="293"/>
+      <c r="E22" s="293"/>
+      <c r="F22" s="293"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="251" t="s">
+      <c r="A23" s="245" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="251" t="s">
+      <c r="B23" s="245" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="251" t="s">
+      <c r="C23" s="245" t="s">
         <v>159</v>
       </c>
-      <c r="D23" s="251" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="251" t="s">
+      <c r="D23" s="245" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="245" t="s">
         <v>160</v>
       </c>
-      <c r="F23" s="252" t="s">
+      <c r="F23" s="246" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="25.5" customHeight="1">
-      <c r="A24" s="251" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" s="245" t="s">
         <v>174</v>
       </c>
-      <c r="B24" s="253"/>
-      <c r="C24" s="253"/>
-      <c r="D24" s="251">
+      <c r="B24" s="247">
+        <v>1</v>
+      </c>
+      <c r="C24" s="247">
+        <v>1</v>
+      </c>
+      <c r="D24" s="245">
         <v>8</v>
       </c>
-      <c r="E24" s="251">
+      <c r="E24" s="245">
         <f t="shared" ref="E24:E34" si="1">B24*C24*D24</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="252"/>
+        <v>8</v>
+      </c>
+      <c r="F24" s="246"/>
+      <c r="G24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="286" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="251" t="s">
+      <c r="A25" s="245" t="s">
         <v>175</v>
       </c>
-      <c r="B25" s="253"/>
-      <c r="C25" s="253"/>
-      <c r="D25" s="251">
+      <c r="B25" s="247">
+        <v>1</v>
+      </c>
+      <c r="C25" s="247">
+        <v>1</v>
+      </c>
+      <c r="D25" s="245">
         <v>16</v>
       </c>
-      <c r="E25" s="251">
+      <c r="E25" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="252"/>
+        <v>16</v>
+      </c>
+      <c r="F25" s="246"/>
+      <c r="G25" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="286"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="251" t="s">
+      <c r="A26" s="245" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="253"/>
-      <c r="C26" s="253"/>
-      <c r="D26" s="251">
+      <c r="B26" s="247">
+        <v>1</v>
+      </c>
+      <c r="C26" s="247">
+        <v>1</v>
+      </c>
+      <c r="D26" s="245">
         <v>8</v>
       </c>
-      <c r="E26" s="251">
+      <c r="E26" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="252"/>
+        <v>8</v>
+      </c>
+      <c r="F26" s="246"/>
+      <c r="G26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="286"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="251" t="s">
+      <c r="A27" s="245" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="253"/>
-      <c r="C27" s="253"/>
-      <c r="D27" s="251">
+      <c r="B27" s="247">
+        <v>1</v>
+      </c>
+      <c r="C27" s="247">
+        <v>1</v>
+      </c>
+      <c r="D27" s="245">
         <v>6</v>
       </c>
-      <c r="E27" s="251">
+      <c r="E27" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="252"/>
+        <v>6</v>
+      </c>
+      <c r="F27" s="246"/>
+      <c r="G27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="286"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="251" t="s">
+      <c r="A28" s="245" t="s">
         <v>178</v>
       </c>
-      <c r="B28" s="253"/>
-      <c r="C28" s="253"/>
-      <c r="D28" s="251">
+      <c r="B28" s="247">
+        <v>1</v>
+      </c>
+      <c r="C28" s="247">
+        <v>1</v>
+      </c>
+      <c r="D28" s="245">
         <v>8</v>
       </c>
-      <c r="E28" s="251">
+      <c r="E28" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="252"/>
+        <v>8</v>
+      </c>
+      <c r="F28" s="246"/>
+      <c r="G28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="286"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="251" t="s">
+      <c r="A29" s="245" t="s">
         <v>179</v>
       </c>
-      <c r="B29" s="253"/>
-      <c r="C29" s="253"/>
-      <c r="D29" s="251">
+      <c r="B29" s="247">
+        <v>1</v>
+      </c>
+      <c r="C29" s="247">
+        <v>1</v>
+      </c>
+      <c r="D29" s="245">
         <v>10</v>
       </c>
-      <c r="E29" s="251">
+      <c r="E29" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="252"/>
+        <v>10</v>
+      </c>
+      <c r="F29" s="246"/>
+      <c r="G29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="286"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="251" t="s">
+      <c r="A30" s="245" t="s">
         <v>180</v>
       </c>
-      <c r="B30" s="253"/>
-      <c r="C30" s="253"/>
-      <c r="D30" s="251">
+      <c r="B30" s="247">
+        <v>1</v>
+      </c>
+      <c r="C30" s="247">
+        <v>1</v>
+      </c>
+      <c r="D30" s="245">
         <v>8</v>
       </c>
-      <c r="E30" s="251">
+      <c r="E30" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="252"/>
+        <v>8</v>
+      </c>
+      <c r="F30" s="246"/>
+      <c r="G30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="286"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="251" t="s">
+      <c r="A31" s="245" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="253"/>
-      <c r="C31" s="253"/>
-      <c r="D31" s="251">
+      <c r="B31" s="247">
+        <v>1</v>
+      </c>
+      <c r="C31" s="247">
+        <v>1</v>
+      </c>
+      <c r="D31" s="245">
         <v>8</v>
       </c>
-      <c r="E31" s="251">
+      <c r="E31" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="252"/>
+        <v>8</v>
+      </c>
+      <c r="F31" s="246"/>
+      <c r="G31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" s="286"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="251" t="s">
+      <c r="A32" s="245" t="s">
         <v>182</v>
       </c>
-      <c r="B32" s="253"/>
-      <c r="C32" s="253"/>
-      <c r="D32" s="251">
+      <c r="B32" s="247">
+        <v>1</v>
+      </c>
+      <c r="C32" s="247">
+        <v>1</v>
+      </c>
+      <c r="D32" s="245">
         <v>8</v>
       </c>
-      <c r="E32" s="251">
+      <c r="E32" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="252"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="251" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="246"/>
+      <c r="G32" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" s="286"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="245" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="253"/>
-      <c r="C33" s="253"/>
-      <c r="D33" s="251">
+      <c r="B33" s="247">
+        <v>1</v>
+      </c>
+      <c r="C33" s="247">
+        <v>0.75</v>
+      </c>
+      <c r="D33" s="245">
         <v>8</v>
       </c>
-      <c r="E33" s="251">
+      <c r="E33" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="252"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="251" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="246"/>
+      <c r="G33" t="s">
+        <v>114</v>
+      </c>
+      <c r="H33" s="286"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="245" t="s">
         <v>184</v>
       </c>
-      <c r="B34" s="253"/>
-      <c r="C34" s="253"/>
-      <c r="D34" s="251">
+      <c r="B34" s="247">
+        <v>1</v>
+      </c>
+      <c r="C34" s="247">
+        <v>1</v>
+      </c>
+      <c r="D34" s="245">
         <v>12</v>
       </c>
-      <c r="E34" s="251">
+      <c r="E34" s="245">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="252"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="254" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="246"/>
+      <c r="G34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" s="286"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="248" t="s">
         <v>171</v>
       </c>
-      <c r="B35" s="254"/>
-      <c r="C35" s="255"/>
-      <c r="D35" s="255">
+      <c r="B35" s="248"/>
+      <c r="C35" s="249"/>
+      <c r="D35" s="249">
         <f>SUM(D24:D34)</f>
         <v>100</v>
       </c>
-      <c r="E35" s="256">
+      <c r="E35" s="250">
         <f>SUM(E24:E34)/D35 -E36*D36 -E37*D37-E38*D38</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="257"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="258" t="s">
+        <v>0.98</v>
+      </c>
+      <c r="F35" s="251"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="252" t="s">
         <v>172</v>
       </c>
-      <c r="C36" s="259"/>
-      <c r="D36" s="260">
+      <c r="C36" s="253"/>
+      <c r="D36" s="254">
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="258" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" s="252" t="s">
         <v>173</v>
       </c>
-      <c r="D37" s="261">
+      <c r="D37" s="255">
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="258" t="s">
+    <row r="38" spans="1:8">
+      <c r="A38" s="252" t="s">
         <v>185</v>
       </c>
-      <c r="D38" s="262">
+      <c r="D38" s="256">
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="23.25">
-      <c r="A39" s="307" t="s">
+    <row r="39" spans="1:8" ht="23.25">
+      <c r="A39" s="294" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="307"/>
-      <c r="C39" s="307"/>
-      <c r="D39" s="307"/>
-      <c r="E39" s="307"/>
-      <c r="F39" s="307"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="263" t="s">
+      <c r="B39" s="294"/>
+      <c r="C39" s="294"/>
+      <c r="D39" s="294"/>
+      <c r="E39" s="294"/>
+      <c r="F39" s="294"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="257" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="308"/>
-      <c r="C40" s="308"/>
-      <c r="D40" s="308"/>
-      <c r="E40" s="308"/>
-      <c r="F40" s="308"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="264" t="s">
+      <c r="B40" s="295"/>
+      <c r="C40" s="295"/>
+      <c r="D40" s="295"/>
+      <c r="E40" s="295"/>
+      <c r="F40" s="295"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="258" t="s">
         <v>158</v>
       </c>
-      <c r="B41" s="265" t="s">
+      <c r="B41" s="259" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="265" t="s">
+      <c r="C41" s="259" t="s">
         <v>159</v>
       </c>
-      <c r="D41" s="265" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="265" t="s">
+      <c r="D41" s="259" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="259" t="s">
         <v>160</v>
       </c>
-      <c r="F41" s="266" t="s">
+      <c r="F41" s="260" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="267" t="s">
+    <row r="42" spans="1:8">
+      <c r="A42" s="261" t="s">
         <v>186</v>
       </c>
-      <c r="B42" s="268"/>
-      <c r="C42" s="268"/>
-      <c r="D42" s="268">
+      <c r="B42" s="262">
+        <v>1</v>
+      </c>
+      <c r="C42" s="262">
+        <v>1</v>
+      </c>
+      <c r="D42" s="262">
         <v>12</v>
       </c>
-      <c r="E42" s="268">
+      <c r="E42" s="262">
         <f t="shared" ref="E42:E51" si="2">B42*C42*D42</f>
-        <v>0</v>
-      </c>
-      <c r="F42" s="266"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="267" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="260"/>
+      <c r="G42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="261" t="s">
         <v>187</v>
       </c>
-      <c r="B43" s="268"/>
-      <c r="C43" s="268"/>
-      <c r="D43" s="268">
+      <c r="B43" s="262">
+        <v>1</v>
+      </c>
+      <c r="C43" s="262">
+        <v>1</v>
+      </c>
+      <c r="D43" s="262">
         <v>16</v>
       </c>
-      <c r="E43" s="268">
+      <c r="E43" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="266"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="267" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="260"/>
+      <c r="G43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="261" t="s">
         <v>188</v>
       </c>
-      <c r="B44" s="268"/>
-      <c r="C44" s="268"/>
-      <c r="D44" s="268">
+      <c r="B44" s="262">
+        <v>0.92</v>
+      </c>
+      <c r="C44" s="262">
+        <v>1</v>
+      </c>
+      <c r="D44" s="262">
         <v>8</v>
       </c>
-      <c r="E44" s="268">
+      <c r="E44" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F44" s="269"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="267" t="s">
+        <v>7.36</v>
+      </c>
+      <c r="F44" s="263"/>
+      <c r="G44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="261" t="s">
         <v>189</v>
       </c>
-      <c r="B45" s="268"/>
-      <c r="C45" s="268"/>
-      <c r="D45" s="268">
+      <c r="B45" s="262">
+        <v>1</v>
+      </c>
+      <c r="C45" s="262">
+        <v>1</v>
+      </c>
+      <c r="D45" s="262">
         <v>12</v>
       </c>
-      <c r="E45" s="268">
+      <c r="E45" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F45" s="266"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="267" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="260"/>
+      <c r="G45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="261" t="s">
         <v>190</v>
       </c>
-      <c r="B46" s="268"/>
-      <c r="C46" s="268"/>
-      <c r="D46" s="268">
+      <c r="B46" s="262">
+        <v>1</v>
+      </c>
+      <c r="C46" s="262">
+        <v>1</v>
+      </c>
+      <c r="D46" s="262">
         <v>10</v>
       </c>
-      <c r="E46" s="268">
+      <c r="E46" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="266"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="267" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="260"/>
+      <c r="G46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="261" t="s">
         <v>191</v>
       </c>
-      <c r="B47" s="268"/>
-      <c r="C47" s="268"/>
-      <c r="D47" s="268">
+      <c r="B47" s="262">
+        <v>1</v>
+      </c>
+      <c r="C47" s="262">
+        <v>1</v>
+      </c>
+      <c r="D47" s="262">
         <v>14</v>
       </c>
-      <c r="E47" s="268">
+      <c r="E47" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F47" s="266"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="270" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="260"/>
+      <c r="G47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="264" t="s">
         <v>192</v>
       </c>
-      <c r="B48" s="268"/>
-      <c r="C48" s="268"/>
-      <c r="D48" s="271">
+      <c r="B48" s="262">
+        <v>1</v>
+      </c>
+      <c r="C48" s="262">
+        <v>1</v>
+      </c>
+      <c r="D48" s="265">
         <v>6</v>
       </c>
-      <c r="E48" s="268">
+      <c r="E48" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="272"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="270" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="266"/>
+      <c r="G48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="264" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="268"/>
-      <c r="C49" s="268"/>
-      <c r="D49" s="271">
+      <c r="B49" s="262">
+        <v>1</v>
+      </c>
+      <c r="C49" s="262">
+        <v>1</v>
+      </c>
+      <c r="D49" s="265">
         <v>8</v>
       </c>
-      <c r="E49" s="268">
+      <c r="E49" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="272"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="270" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="266"/>
+      <c r="G49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="264" t="s">
         <v>194</v>
       </c>
-      <c r="B50" s="268"/>
-      <c r="C50" s="268"/>
-      <c r="D50" s="271">
+      <c r="B50" s="262">
+        <v>1</v>
+      </c>
+      <c r="C50" s="262">
+        <v>1</v>
+      </c>
+      <c r="D50" s="265">
         <v>6</v>
       </c>
-      <c r="E50" s="268">
+      <c r="E50" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="272"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="270" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="266"/>
+      <c r="G50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="264" t="s">
         <v>195</v>
       </c>
-      <c r="B51" s="268"/>
-      <c r="C51" s="268"/>
-      <c r="D51" s="271">
+      <c r="B51" s="262">
+        <v>1</v>
+      </c>
+      <c r="C51" s="262">
+        <v>1</v>
+      </c>
+      <c r="D51" s="265">
         <v>8</v>
       </c>
-      <c r="E51" s="268">
+      <c r="E51" s="262">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="272"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="273" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="266"/>
+      <c r="G51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="267" t="s">
         <v>171</v>
       </c>
-      <c r="B52" s="274"/>
-      <c r="C52" s="274"/>
-      <c r="D52" s="275">
+      <c r="B52" s="268"/>
+      <c r="C52" s="268"/>
+      <c r="D52" s="269">
         <f>SUM(D42:D51)</f>
         <v>100</v>
       </c>
-      <c r="E52" s="276">
+      <c r="E52" s="270">
         <f>SUM(E42:E51)/D52 - D53*E53  - D54*E54 - D55*E55</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="277"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="278" t="s">
+        <v>0.99360000000000004</v>
+      </c>
+      <c r="F52" s="271"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="272" t="s">
         <v>172</v>
       </c>
-      <c r="D53" s="261">
+      <c r="D53" s="255">
         <v>0.15</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="278" t="s">
+    <row r="54" spans="1:7">
+      <c r="A54" s="272" t="s">
         <v>173</v>
       </c>
-      <c r="D54" s="261">
+      <c r="D54" s="255">
         <v>0.2</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="279" t="s">
+    <row r="55" spans="1:7">
+      <c r="A55" s="273" t="s">
         <v>185</v>
       </c>
-      <c r="D55" s="262">
+      <c r="D55" s="256">
         <v>0.05</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="H8:H17"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="B40:F40"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H24:H34"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B18 B42:B51" xr:uid="{00000000-0002-0000-0700-000000000000}">

</xml_diff>